<commit_message>
Manufacturing documents for the beta trials
</commit_message>
<xml_diff>
--- a/bom/electron-bom-v010-150805.xlsx
+++ b/bom/electron-bom-v010-150805.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ELECTRON" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="TBD" sheetId="6" r:id="rId3"/>
     <sheet name="CHANGELOG" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1778,39 +1778,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1881,6 +1848,39 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2241,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HL958"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
@@ -3491,19 +3491,19 @@
       </c>
       <c r="G41" s="63"/>
       <c r="H41" s="70"/>
-      <c r="I41" s="87" t="s">
+      <c r="I41" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="J41" s="87" t="s">
+      <c r="J41" s="74" t="s">
         <v>65</v>
       </c>
       <c r="K41" s="72">
         <v>1</v>
       </c>
-      <c r="L41" s="87" t="s">
+      <c r="L41" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="M41" s="87" t="s">
+      <c r="M41" s="74" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3598,52 +3598,52 @@
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B45" s="90" t="s">
+      <c r="B45" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="90" t="s">
+      <c r="C45" s="77" t="s">
         <v>315</v>
       </c>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="90" t="s">
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="77" t="s">
         <v>316</v>
       </c>
-      <c r="J45" s="92"/>
-      <c r="K45" s="95">
+      <c r="J45" s="79"/>
+      <c r="K45" s="82">
         <v>1</v>
       </c>
-      <c r="L45" s="93" t="s">
+      <c r="L45" s="80" t="s">
         <v>317</v>
       </c>
-      <c r="M45" s="94"/>
+      <c r="M45" s="81"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.15">
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="C46" s="90" t="s">
+      <c r="C46" s="77" t="s">
         <v>336</v>
       </c>
-      <c r="D46" s="91"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="91"/>
-      <c r="G46" s="91"/>
-      <c r="H46" s="91"/>
-      <c r="I46" s="90" t="s">
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="77" t="s">
         <v>316</v>
       </c>
-      <c r="J46" s="92"/>
-      <c r="K46" s="95">
+      <c r="J46" s="79"/>
+      <c r="K46" s="82">
         <v>1</v>
       </c>
-      <c r="L46" s="93" t="s">
+      <c r="L46" s="80" t="s">
         <v>318</v>
       </c>
-      <c r="M46" s="94"/>
+      <c r="M46" s="81"/>
     </row>
     <row r="47" spans="2:13" ht="26" x14ac:dyDescent="0.15">
       <c r="B47" s="18" t="s">
@@ -17046,10 +17046,10 @@
       <c r="K6" s="19">
         <v>1</v>
       </c>
-      <c r="L6" s="88" t="s">
+      <c r="L6" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="89" t="s">
+      <c r="M6" s="76" t="s">
         <v>309</v>
       </c>
     </row>
@@ -17074,10 +17074,10 @@
       <c r="K7" s="19">
         <v>1</v>
       </c>
-      <c r="L7" s="88" t="s">
+      <c r="L7" s="75" t="s">
         <v>167</v>
       </c>
-      <c r="M7" s="89"/>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B8" s="18" t="s">
@@ -17100,8 +17100,8 @@
       <c r="K8" s="19">
         <v>1</v>
       </c>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B9" s="18" t="s">
@@ -17124,8 +17124,8 @@
       <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B10" s="16"/>
@@ -29359,7 +29359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IF881"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -29466,1528 +29466,1528 @@
       </c>
     </row>
     <row r="5" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="85"/>
+      <c r="B5" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="87" t="s">
         <v>337</v>
       </c>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="101"/>
-      <c r="I5" s="100" t="s">
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="87" t="s">
         <v>316</v>
       </c>
-      <c r="J5" s="100"/>
-      <c r="K5" s="102">
+      <c r="J5" s="87"/>
+      <c r="K5" s="89">
         <v>1</v>
       </c>
-      <c r="L5" s="103" t="s">
+      <c r="L5" s="90" t="s">
         <v>167</v>
       </c>
-      <c r="M5" s="104"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="96"/>
-      <c r="X5" s="96"/>
-      <c r="Y5" s="96"/>
-      <c r="Z5" s="96"/>
-      <c r="AA5" s="96"/>
-      <c r="AB5" s="96"/>
-      <c r="AC5" s="96"/>
-      <c r="AD5" s="96"/>
-      <c r="AE5" s="96"/>
-      <c r="AF5" s="96"/>
-      <c r="AG5" s="96"/>
-      <c r="AH5" s="96"/>
-      <c r="AI5" s="96"/>
-      <c r="AJ5" s="96"/>
-      <c r="AK5" s="96"/>
-      <c r="AL5" s="96"/>
-      <c r="AM5" s="96"/>
-      <c r="AN5" s="96"/>
-      <c r="AO5" s="96"/>
-      <c r="AP5" s="96"/>
-      <c r="AQ5" s="96"/>
-      <c r="AR5" s="96"/>
-      <c r="AS5" s="96"/>
-      <c r="AT5" s="96"/>
-      <c r="AU5" s="96"/>
-      <c r="AV5" s="96"/>
-      <c r="AW5" s="96"/>
-      <c r="AX5" s="96"/>
-      <c r="AY5" s="96"/>
-      <c r="AZ5" s="96"/>
-      <c r="BA5" s="96"/>
-      <c r="BB5" s="96"/>
-      <c r="BC5" s="96"/>
-      <c r="BD5" s="96"/>
-      <c r="BE5" s="96"/>
-      <c r="BF5" s="96"/>
-      <c r="BG5" s="96"/>
-      <c r="BH5" s="96"/>
-      <c r="BI5" s="96"/>
-      <c r="BJ5" s="96"/>
-      <c r="BK5" s="96"/>
-      <c r="BL5" s="96"/>
-      <c r="BM5" s="96"/>
-      <c r="BN5" s="96"/>
-      <c r="BO5" s="96"/>
-      <c r="BP5" s="96"/>
-      <c r="BQ5" s="96"/>
-      <c r="BR5" s="96"/>
-      <c r="BS5" s="96"/>
-      <c r="BT5" s="96"/>
-      <c r="BU5" s="96"/>
-      <c r="BV5" s="96"/>
-      <c r="BW5" s="96"/>
-      <c r="BX5" s="96"/>
-      <c r="BY5" s="96"/>
-      <c r="BZ5" s="96"/>
-      <c r="CA5" s="96"/>
-      <c r="CB5" s="96"/>
-      <c r="CC5" s="96"/>
-      <c r="CD5" s="96"/>
-      <c r="CE5" s="96"/>
-      <c r="CF5" s="96"/>
-      <c r="CG5" s="96"/>
-      <c r="CH5" s="96"/>
-      <c r="CI5" s="96"/>
-      <c r="CJ5" s="96"/>
-      <c r="CK5" s="96"/>
-      <c r="CL5" s="96"/>
-      <c r="CM5" s="96"/>
-      <c r="CN5" s="96"/>
-      <c r="CO5" s="96"/>
-      <c r="CP5" s="96"/>
-      <c r="CQ5" s="96"/>
-      <c r="CR5" s="96"/>
-      <c r="CS5" s="96"/>
-      <c r="CT5" s="96"/>
-      <c r="CU5" s="96"/>
-      <c r="CV5" s="96"/>
-      <c r="CW5" s="96"/>
-      <c r="CX5" s="96"/>
-      <c r="CY5" s="96"/>
-      <c r="CZ5" s="96"/>
-      <c r="DA5" s="96"/>
-      <c r="DB5" s="96"/>
-      <c r="DC5" s="96"/>
-      <c r="DD5" s="96"/>
-      <c r="DE5" s="96"/>
-      <c r="DF5" s="96"/>
-      <c r="DG5" s="96"/>
-      <c r="DH5" s="96"/>
-      <c r="DI5" s="96"/>
-      <c r="DJ5" s="96"/>
-      <c r="DK5" s="96"/>
-      <c r="DL5" s="96"/>
-      <c r="DM5" s="96"/>
-      <c r="DN5" s="96"/>
-      <c r="DO5" s="96"/>
-      <c r="DP5" s="96"/>
-      <c r="DQ5" s="96"/>
-      <c r="DR5" s="96"/>
-      <c r="DS5" s="96"/>
-      <c r="DT5" s="96"/>
-      <c r="DU5" s="96"/>
-      <c r="DV5" s="96"/>
-      <c r="DW5" s="96"/>
-      <c r="DX5" s="96"/>
-      <c r="DY5" s="96"/>
-      <c r="DZ5" s="96"/>
-      <c r="EA5" s="96"/>
-      <c r="EB5" s="96"/>
-      <c r="EC5" s="96"/>
-      <c r="ED5" s="96"/>
-      <c r="EE5" s="96"/>
-      <c r="EF5" s="96"/>
-      <c r="EG5" s="96"/>
-      <c r="EH5" s="96"/>
-      <c r="EI5" s="96"/>
-      <c r="EJ5" s="96"/>
-      <c r="EK5" s="96"/>
-      <c r="EL5" s="96"/>
-      <c r="EM5" s="96"/>
-      <c r="EN5" s="96"/>
-      <c r="EO5" s="96"/>
-      <c r="EP5" s="96"/>
-      <c r="EQ5" s="96"/>
-      <c r="ER5" s="96"/>
-      <c r="ES5" s="96"/>
-      <c r="ET5" s="96"/>
-      <c r="EU5" s="96"/>
-      <c r="EV5" s="96"/>
-      <c r="EW5" s="96"/>
-      <c r="EX5" s="96"/>
-      <c r="EY5" s="96"/>
-      <c r="EZ5" s="96"/>
-      <c r="FA5" s="96"/>
-      <c r="FB5" s="96"/>
-      <c r="FC5" s="96"/>
-      <c r="FD5" s="96"/>
-      <c r="FE5" s="96"/>
-      <c r="FF5" s="96"/>
-      <c r="FG5" s="96"/>
-      <c r="FH5" s="96"/>
-      <c r="FI5" s="96"/>
-      <c r="FJ5" s="96"/>
-      <c r="FK5" s="96"/>
-      <c r="FL5" s="96"/>
-      <c r="FM5" s="96"/>
-      <c r="FN5" s="96"/>
-      <c r="FO5" s="96"/>
-      <c r="FP5" s="96"/>
-      <c r="FQ5" s="96"/>
-      <c r="FR5" s="96"/>
-      <c r="FS5" s="96"/>
-      <c r="FT5" s="96"/>
-      <c r="FU5" s="96"/>
-      <c r="FV5" s="96"/>
-      <c r="FW5" s="96"/>
-      <c r="FX5" s="96"/>
-      <c r="FY5" s="96"/>
-      <c r="FZ5" s="96"/>
-      <c r="GA5" s="96"/>
-      <c r="GB5" s="96"/>
-      <c r="GC5" s="96"/>
-      <c r="GD5" s="96"/>
-      <c r="GE5" s="96"/>
-      <c r="GF5" s="96"/>
-      <c r="GG5" s="96"/>
-      <c r="GH5" s="96"/>
-      <c r="GI5" s="96"/>
-      <c r="GJ5" s="96"/>
-      <c r="GK5" s="96"/>
-      <c r="GL5" s="96"/>
-      <c r="GM5" s="96"/>
-      <c r="GN5" s="96"/>
-      <c r="GO5" s="96"/>
-      <c r="GP5" s="96"/>
-      <c r="GQ5" s="96"/>
-      <c r="GR5" s="96"/>
-      <c r="GS5" s="96"/>
-      <c r="GT5" s="96"/>
-      <c r="GU5" s="96"/>
-      <c r="GV5" s="96"/>
-      <c r="GW5" s="96"/>
-      <c r="GX5" s="96"/>
-      <c r="GY5" s="96"/>
-      <c r="GZ5" s="96"/>
-      <c r="HA5" s="96"/>
-      <c r="HB5" s="96"/>
-      <c r="HC5" s="96"/>
-      <c r="HD5" s="96"/>
-      <c r="HE5" s="96"/>
-      <c r="HF5" s="96"/>
-      <c r="HG5" s="96"/>
-      <c r="HH5" s="96"/>
-      <c r="HI5" s="96"/>
-      <c r="HJ5" s="96"/>
-      <c r="HK5" s="96"/>
-      <c r="HL5" s="96"/>
-      <c r="HM5" s="96"/>
-      <c r="HN5" s="96"/>
-      <c r="HO5" s="96"/>
-      <c r="HP5" s="96"/>
-      <c r="HQ5" s="96"/>
-      <c r="HR5" s="96"/>
-      <c r="HS5" s="96"/>
-      <c r="HT5" s="96"/>
-      <c r="HU5" s="96"/>
-      <c r="HV5" s="96"/>
-      <c r="HW5" s="96"/>
-      <c r="HX5" s="96"/>
-      <c r="HY5" s="96"/>
-      <c r="HZ5" s="96"/>
-      <c r="IA5" s="96"/>
-      <c r="IB5" s="96"/>
-      <c r="IC5" s="96"/>
-      <c r="ID5" s="96"/>
-      <c r="IE5" s="96"/>
-      <c r="IF5" s="96"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="83"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="83"/>
+      <c r="AH5" s="83"/>
+      <c r="AI5" s="83"/>
+      <c r="AJ5" s="83"/>
+      <c r="AK5" s="83"/>
+      <c r="AL5" s="83"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="83"/>
+      <c r="AO5" s="83"/>
+      <c r="AP5" s="83"/>
+      <c r="AQ5" s="83"/>
+      <c r="AR5" s="83"/>
+      <c r="AS5" s="83"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="83"/>
+      <c r="AV5" s="83"/>
+      <c r="AW5" s="83"/>
+      <c r="AX5" s="83"/>
+      <c r="AY5" s="83"/>
+      <c r="AZ5" s="83"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="83"/>
+      <c r="BC5" s="83"/>
+      <c r="BD5" s="83"/>
+      <c r="BE5" s="83"/>
+      <c r="BF5" s="83"/>
+      <c r="BG5" s="83"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="83"/>
+      <c r="BJ5" s="83"/>
+      <c r="BK5" s="83"/>
+      <c r="BL5" s="83"/>
+      <c r="BM5" s="83"/>
+      <c r="BN5" s="83"/>
+      <c r="BO5" s="83"/>
+      <c r="BP5" s="83"/>
+      <c r="BQ5" s="83"/>
+      <c r="BR5" s="83"/>
+      <c r="BS5" s="83"/>
+      <c r="BT5" s="83"/>
+      <c r="BU5" s="83"/>
+      <c r="BV5" s="83"/>
+      <c r="BW5" s="83"/>
+      <c r="BX5" s="83"/>
+      <c r="BY5" s="83"/>
+      <c r="BZ5" s="83"/>
+      <c r="CA5" s="83"/>
+      <c r="CB5" s="83"/>
+      <c r="CC5" s="83"/>
+      <c r="CD5" s="83"/>
+      <c r="CE5" s="83"/>
+      <c r="CF5" s="83"/>
+      <c r="CG5" s="83"/>
+      <c r="CH5" s="83"/>
+      <c r="CI5" s="83"/>
+      <c r="CJ5" s="83"/>
+      <c r="CK5" s="83"/>
+      <c r="CL5" s="83"/>
+      <c r="CM5" s="83"/>
+      <c r="CN5" s="83"/>
+      <c r="CO5" s="83"/>
+      <c r="CP5" s="83"/>
+      <c r="CQ5" s="83"/>
+      <c r="CR5" s="83"/>
+      <c r="CS5" s="83"/>
+      <c r="CT5" s="83"/>
+      <c r="CU5" s="83"/>
+      <c r="CV5" s="83"/>
+      <c r="CW5" s="83"/>
+      <c r="CX5" s="83"/>
+      <c r="CY5" s="83"/>
+      <c r="CZ5" s="83"/>
+      <c r="DA5" s="83"/>
+      <c r="DB5" s="83"/>
+      <c r="DC5" s="83"/>
+      <c r="DD5" s="83"/>
+      <c r="DE5" s="83"/>
+      <c r="DF5" s="83"/>
+      <c r="DG5" s="83"/>
+      <c r="DH5" s="83"/>
+      <c r="DI5" s="83"/>
+      <c r="DJ5" s="83"/>
+      <c r="DK5" s="83"/>
+      <c r="DL5" s="83"/>
+      <c r="DM5" s="83"/>
+      <c r="DN5" s="83"/>
+      <c r="DO5" s="83"/>
+      <c r="DP5" s="83"/>
+      <c r="DQ5" s="83"/>
+      <c r="DR5" s="83"/>
+      <c r="DS5" s="83"/>
+      <c r="DT5" s="83"/>
+      <c r="DU5" s="83"/>
+      <c r="DV5" s="83"/>
+      <c r="DW5" s="83"/>
+      <c r="DX5" s="83"/>
+      <c r="DY5" s="83"/>
+      <c r="DZ5" s="83"/>
+      <c r="EA5" s="83"/>
+      <c r="EB5" s="83"/>
+      <c r="EC5" s="83"/>
+      <c r="ED5" s="83"/>
+      <c r="EE5" s="83"/>
+      <c r="EF5" s="83"/>
+      <c r="EG5" s="83"/>
+      <c r="EH5" s="83"/>
+      <c r="EI5" s="83"/>
+      <c r="EJ5" s="83"/>
+      <c r="EK5" s="83"/>
+      <c r="EL5" s="83"/>
+      <c r="EM5" s="83"/>
+      <c r="EN5" s="83"/>
+      <c r="EO5" s="83"/>
+      <c r="EP5" s="83"/>
+      <c r="EQ5" s="83"/>
+      <c r="ER5" s="83"/>
+      <c r="ES5" s="83"/>
+      <c r="ET5" s="83"/>
+      <c r="EU5" s="83"/>
+      <c r="EV5" s="83"/>
+      <c r="EW5" s="83"/>
+      <c r="EX5" s="83"/>
+      <c r="EY5" s="83"/>
+      <c r="EZ5" s="83"/>
+      <c r="FA5" s="83"/>
+      <c r="FB5" s="83"/>
+      <c r="FC5" s="83"/>
+      <c r="FD5" s="83"/>
+      <c r="FE5" s="83"/>
+      <c r="FF5" s="83"/>
+      <c r="FG5" s="83"/>
+      <c r="FH5" s="83"/>
+      <c r="FI5" s="83"/>
+      <c r="FJ5" s="83"/>
+      <c r="FK5" s="83"/>
+      <c r="FL5" s="83"/>
+      <c r="FM5" s="83"/>
+      <c r="FN5" s="83"/>
+      <c r="FO5" s="83"/>
+      <c r="FP5" s="83"/>
+      <c r="FQ5" s="83"/>
+      <c r="FR5" s="83"/>
+      <c r="FS5" s="83"/>
+      <c r="FT5" s="83"/>
+      <c r="FU5" s="83"/>
+      <c r="FV5" s="83"/>
+      <c r="FW5" s="83"/>
+      <c r="FX5" s="83"/>
+      <c r="FY5" s="83"/>
+      <c r="FZ5" s="83"/>
+      <c r="GA5" s="83"/>
+      <c r="GB5" s="83"/>
+      <c r="GC5" s="83"/>
+      <c r="GD5" s="83"/>
+      <c r="GE5" s="83"/>
+      <c r="GF5" s="83"/>
+      <c r="GG5" s="83"/>
+      <c r="GH5" s="83"/>
+      <c r="GI5" s="83"/>
+      <c r="GJ5" s="83"/>
+      <c r="GK5" s="83"/>
+      <c r="GL5" s="83"/>
+      <c r="GM5" s="83"/>
+      <c r="GN5" s="83"/>
+      <c r="GO5" s="83"/>
+      <c r="GP5" s="83"/>
+      <c r="GQ5" s="83"/>
+      <c r="GR5" s="83"/>
+      <c r="GS5" s="83"/>
+      <c r="GT5" s="83"/>
+      <c r="GU5" s="83"/>
+      <c r="GV5" s="83"/>
+      <c r="GW5" s="83"/>
+      <c r="GX5" s="83"/>
+      <c r="GY5" s="83"/>
+      <c r="GZ5" s="83"/>
+      <c r="HA5" s="83"/>
+      <c r="HB5" s="83"/>
+      <c r="HC5" s="83"/>
+      <c r="HD5" s="83"/>
+      <c r="HE5" s="83"/>
+      <c r="HF5" s="83"/>
+      <c r="HG5" s="83"/>
+      <c r="HH5" s="83"/>
+      <c r="HI5" s="83"/>
+      <c r="HJ5" s="83"/>
+      <c r="HK5" s="83"/>
+      <c r="HL5" s="83"/>
+      <c r="HM5" s="83"/>
+      <c r="HN5" s="83"/>
+      <c r="HO5" s="83"/>
+      <c r="HP5" s="83"/>
+      <c r="HQ5" s="83"/>
+      <c r="HR5" s="83"/>
+      <c r="HS5" s="83"/>
+      <c r="HT5" s="83"/>
+      <c r="HU5" s="83"/>
+      <c r="HV5" s="83"/>
+      <c r="HW5" s="83"/>
+      <c r="HX5" s="83"/>
+      <c r="HY5" s="83"/>
+      <c r="HZ5" s="83"/>
+      <c r="IA5" s="83"/>
+      <c r="IB5" s="83"/>
+      <c r="IC5" s="83"/>
+      <c r="ID5" s="83"/>
+      <c r="IE5" s="83"/>
+      <c r="IF5" s="83"/>
     </row>
     <row r="6" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A6" s="98"/>
-      <c r="B6" s="107" t="s">
+      <c r="A6" s="85"/>
+      <c r="B6" s="94" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="95" t="s">
         <v>319</v>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="108" t="s">
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="95" t="s">
         <v>316</v>
       </c>
-      <c r="J6" s="108"/>
-      <c r="K6" s="110">
+      <c r="J6" s="95"/>
+      <c r="K6" s="97">
         <v>1</v>
       </c>
-      <c r="L6" s="108" t="s">
+      <c r="L6" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="111"/>
-      <c r="N6" s="97"/>
-      <c r="O6" s="97"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="96"/>
-      <c r="U6" s="96"/>
-      <c r="V6" s="96"/>
-      <c r="W6" s="96"/>
-      <c r="X6" s="96"/>
-      <c r="Y6" s="96"/>
-      <c r="Z6" s="96"/>
-      <c r="AA6" s="96"/>
-      <c r="AB6" s="96"/>
-      <c r="AC6" s="96"/>
-      <c r="AD6" s="96"/>
-      <c r="AE6" s="96"/>
-      <c r="AF6" s="96"/>
-      <c r="AG6" s="96"/>
-      <c r="AH6" s="96"/>
-      <c r="AI6" s="96"/>
-      <c r="AJ6" s="96"/>
-      <c r="AK6" s="96"/>
-      <c r="AL6" s="96"/>
-      <c r="AM6" s="96"/>
-      <c r="AN6" s="96"/>
-      <c r="AO6" s="96"/>
-      <c r="AP6" s="96"/>
-      <c r="AQ6" s="96"/>
-      <c r="AR6" s="96"/>
-      <c r="AS6" s="96"/>
-      <c r="AT6" s="96"/>
-      <c r="AU6" s="96"/>
-      <c r="AV6" s="96"/>
-      <c r="AW6" s="96"/>
-      <c r="AX6" s="96"/>
-      <c r="AY6" s="96"/>
-      <c r="AZ6" s="96"/>
-      <c r="BA6" s="96"/>
-      <c r="BB6" s="96"/>
-      <c r="BC6" s="96"/>
-      <c r="BD6" s="96"/>
-      <c r="BE6" s="96"/>
-      <c r="BF6" s="96"/>
-      <c r="BG6" s="96"/>
-      <c r="BH6" s="96"/>
-      <c r="BI6" s="96"/>
-      <c r="BJ6" s="96"/>
-      <c r="BK6" s="96"/>
-      <c r="BL6" s="96"/>
-      <c r="BM6" s="96"/>
-      <c r="BN6" s="96"/>
-      <c r="BO6" s="96"/>
-      <c r="BP6" s="96"/>
-      <c r="BQ6" s="96"/>
-      <c r="BR6" s="96"/>
-      <c r="BS6" s="96"/>
-      <c r="BT6" s="96"/>
-      <c r="BU6" s="96"/>
-      <c r="BV6" s="96"/>
-      <c r="BW6" s="96"/>
-      <c r="BX6" s="96"/>
-      <c r="BY6" s="96"/>
-      <c r="BZ6" s="96"/>
-      <c r="CA6" s="96"/>
-      <c r="CB6" s="96"/>
-      <c r="CC6" s="96"/>
-      <c r="CD6" s="96"/>
-      <c r="CE6" s="96"/>
-      <c r="CF6" s="96"/>
-      <c r="CG6" s="96"/>
-      <c r="CH6" s="96"/>
-      <c r="CI6" s="96"/>
-      <c r="CJ6" s="96"/>
-      <c r="CK6" s="96"/>
-      <c r="CL6" s="96"/>
-      <c r="CM6" s="96"/>
-      <c r="CN6" s="96"/>
-      <c r="CO6" s="96"/>
-      <c r="CP6" s="96"/>
-      <c r="CQ6" s="96"/>
-      <c r="CR6" s="96"/>
-      <c r="CS6" s="96"/>
-      <c r="CT6" s="96"/>
-      <c r="CU6" s="96"/>
-      <c r="CV6" s="96"/>
-      <c r="CW6" s="96"/>
-      <c r="CX6" s="96"/>
-      <c r="CY6" s="96"/>
-      <c r="CZ6" s="96"/>
-      <c r="DA6" s="96"/>
-      <c r="DB6" s="96"/>
-      <c r="DC6" s="96"/>
-      <c r="DD6" s="96"/>
-      <c r="DE6" s="96"/>
-      <c r="DF6" s="96"/>
-      <c r="DG6" s="96"/>
-      <c r="DH6" s="96"/>
-      <c r="DI6" s="96"/>
-      <c r="DJ6" s="96"/>
-      <c r="DK6" s="96"/>
-      <c r="DL6" s="96"/>
-      <c r="DM6" s="96"/>
-      <c r="DN6" s="96"/>
-      <c r="DO6" s="96"/>
-      <c r="DP6" s="96"/>
-      <c r="DQ6" s="96"/>
-      <c r="DR6" s="96"/>
-      <c r="DS6" s="96"/>
-      <c r="DT6" s="96"/>
-      <c r="DU6" s="96"/>
-      <c r="DV6" s="96"/>
-      <c r="DW6" s="96"/>
-      <c r="DX6" s="96"/>
-      <c r="DY6" s="96"/>
-      <c r="DZ6" s="96"/>
-      <c r="EA6" s="96"/>
-      <c r="EB6" s="96"/>
-      <c r="EC6" s="96"/>
-      <c r="ED6" s="96"/>
-      <c r="EE6" s="96"/>
-      <c r="EF6" s="96"/>
-      <c r="EG6" s="96"/>
-      <c r="EH6" s="96"/>
-      <c r="EI6" s="96"/>
-      <c r="EJ6" s="96"/>
-      <c r="EK6" s="96"/>
-      <c r="EL6" s="96"/>
-      <c r="EM6" s="96"/>
-      <c r="EN6" s="96"/>
-      <c r="EO6" s="96"/>
-      <c r="EP6" s="96"/>
-      <c r="EQ6" s="96"/>
-      <c r="ER6" s="96"/>
-      <c r="ES6" s="96"/>
-      <c r="ET6" s="96"/>
-      <c r="EU6" s="96"/>
-      <c r="EV6" s="96"/>
-      <c r="EW6" s="96"/>
-      <c r="EX6" s="96"/>
-      <c r="EY6" s="96"/>
-      <c r="EZ6" s="96"/>
-      <c r="FA6" s="96"/>
-      <c r="FB6" s="96"/>
-      <c r="FC6" s="96"/>
-      <c r="FD6" s="96"/>
-      <c r="FE6" s="96"/>
-      <c r="FF6" s="96"/>
-      <c r="FG6" s="96"/>
-      <c r="FH6" s="96"/>
-      <c r="FI6" s="96"/>
-      <c r="FJ6" s="96"/>
-      <c r="FK6" s="96"/>
-      <c r="FL6" s="96"/>
-      <c r="FM6" s="96"/>
-      <c r="FN6" s="96"/>
-      <c r="FO6" s="96"/>
-      <c r="FP6" s="96"/>
-      <c r="FQ6" s="96"/>
-      <c r="FR6" s="96"/>
-      <c r="FS6" s="96"/>
-      <c r="FT6" s="96"/>
-      <c r="FU6" s="96"/>
-      <c r="FV6" s="96"/>
-      <c r="FW6" s="96"/>
-      <c r="FX6" s="96"/>
-      <c r="FY6" s="96"/>
-      <c r="FZ6" s="96"/>
-      <c r="GA6" s="96"/>
-      <c r="GB6" s="96"/>
-      <c r="GC6" s="96"/>
-      <c r="GD6" s="96"/>
-      <c r="GE6" s="96"/>
-      <c r="GF6" s="96"/>
-      <c r="GG6" s="96"/>
-      <c r="GH6" s="96"/>
-      <c r="GI6" s="96"/>
-      <c r="GJ6" s="96"/>
-      <c r="GK6" s="96"/>
-      <c r="GL6" s="96"/>
-      <c r="GM6" s="96"/>
-      <c r="GN6" s="96"/>
-      <c r="GO6" s="96"/>
-      <c r="GP6" s="96"/>
-      <c r="GQ6" s="96"/>
-      <c r="GR6" s="96"/>
-      <c r="GS6" s="96"/>
-      <c r="GT6" s="96"/>
-      <c r="GU6" s="96"/>
-      <c r="GV6" s="96"/>
-      <c r="GW6" s="96"/>
-      <c r="GX6" s="96"/>
-      <c r="GY6" s="96"/>
-      <c r="GZ6" s="96"/>
-      <c r="HA6" s="96"/>
-      <c r="HB6" s="96"/>
-      <c r="HC6" s="96"/>
-      <c r="HD6" s="96"/>
-      <c r="HE6" s="96"/>
-      <c r="HF6" s="96"/>
-      <c r="HG6" s="96"/>
-      <c r="HH6" s="96"/>
-      <c r="HI6" s="96"/>
-      <c r="HJ6" s="96"/>
-      <c r="HK6" s="96"/>
-      <c r="HL6" s="96"/>
-      <c r="HM6" s="96"/>
-      <c r="HN6" s="96"/>
-      <c r="HO6" s="96"/>
-      <c r="HP6" s="96"/>
-      <c r="HQ6" s="96"/>
-      <c r="HR6" s="96"/>
-      <c r="HS6" s="96"/>
-      <c r="HT6" s="96"/>
-      <c r="HU6" s="96"/>
-      <c r="HV6" s="96"/>
-      <c r="HW6" s="96"/>
-      <c r="HX6" s="96"/>
-      <c r="HY6" s="96"/>
-      <c r="HZ6" s="96"/>
-      <c r="IA6" s="96"/>
-      <c r="IB6" s="96"/>
-      <c r="IC6" s="96"/>
-      <c r="ID6" s="96"/>
-      <c r="IE6" s="96"/>
-      <c r="IF6" s="96"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="84"/>
+      <c r="P6" s="92"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="83"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="83"/>
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="83"/>
+      <c r="AF6" s="83"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="83"/>
+      <c r="AI6" s="83"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="83"/>
+      <c r="AL6" s="83"/>
+      <c r="AM6" s="83"/>
+      <c r="AN6" s="83"/>
+      <c r="AO6" s="83"/>
+      <c r="AP6" s="83"/>
+      <c r="AQ6" s="83"/>
+      <c r="AR6" s="83"/>
+      <c r="AS6" s="83"/>
+      <c r="AT6" s="83"/>
+      <c r="AU6" s="83"/>
+      <c r="AV6" s="83"/>
+      <c r="AW6" s="83"/>
+      <c r="AX6" s="83"/>
+      <c r="AY6" s="83"/>
+      <c r="AZ6" s="83"/>
+      <c r="BA6" s="83"/>
+      <c r="BB6" s="83"/>
+      <c r="BC6" s="83"/>
+      <c r="BD6" s="83"/>
+      <c r="BE6" s="83"/>
+      <c r="BF6" s="83"/>
+      <c r="BG6" s="83"/>
+      <c r="BH6" s="83"/>
+      <c r="BI6" s="83"/>
+      <c r="BJ6" s="83"/>
+      <c r="BK6" s="83"/>
+      <c r="BL6" s="83"/>
+      <c r="BM6" s="83"/>
+      <c r="BN6" s="83"/>
+      <c r="BO6" s="83"/>
+      <c r="BP6" s="83"/>
+      <c r="BQ6" s="83"/>
+      <c r="BR6" s="83"/>
+      <c r="BS6" s="83"/>
+      <c r="BT6" s="83"/>
+      <c r="BU6" s="83"/>
+      <c r="BV6" s="83"/>
+      <c r="BW6" s="83"/>
+      <c r="BX6" s="83"/>
+      <c r="BY6" s="83"/>
+      <c r="BZ6" s="83"/>
+      <c r="CA6" s="83"/>
+      <c r="CB6" s="83"/>
+      <c r="CC6" s="83"/>
+      <c r="CD6" s="83"/>
+      <c r="CE6" s="83"/>
+      <c r="CF6" s="83"/>
+      <c r="CG6" s="83"/>
+      <c r="CH6" s="83"/>
+      <c r="CI6" s="83"/>
+      <c r="CJ6" s="83"/>
+      <c r="CK6" s="83"/>
+      <c r="CL6" s="83"/>
+      <c r="CM6" s="83"/>
+      <c r="CN6" s="83"/>
+      <c r="CO6" s="83"/>
+      <c r="CP6" s="83"/>
+      <c r="CQ6" s="83"/>
+      <c r="CR6" s="83"/>
+      <c r="CS6" s="83"/>
+      <c r="CT6" s="83"/>
+      <c r="CU6" s="83"/>
+      <c r="CV6" s="83"/>
+      <c r="CW6" s="83"/>
+      <c r="CX6" s="83"/>
+      <c r="CY6" s="83"/>
+      <c r="CZ6" s="83"/>
+      <c r="DA6" s="83"/>
+      <c r="DB6" s="83"/>
+      <c r="DC6" s="83"/>
+      <c r="DD6" s="83"/>
+      <c r="DE6" s="83"/>
+      <c r="DF6" s="83"/>
+      <c r="DG6" s="83"/>
+      <c r="DH6" s="83"/>
+      <c r="DI6" s="83"/>
+      <c r="DJ6" s="83"/>
+      <c r="DK6" s="83"/>
+      <c r="DL6" s="83"/>
+      <c r="DM6" s="83"/>
+      <c r="DN6" s="83"/>
+      <c r="DO6" s="83"/>
+      <c r="DP6" s="83"/>
+      <c r="DQ6" s="83"/>
+      <c r="DR6" s="83"/>
+      <c r="DS6" s="83"/>
+      <c r="DT6" s="83"/>
+      <c r="DU6" s="83"/>
+      <c r="DV6" s="83"/>
+      <c r="DW6" s="83"/>
+      <c r="DX6" s="83"/>
+      <c r="DY6" s="83"/>
+      <c r="DZ6" s="83"/>
+      <c r="EA6" s="83"/>
+      <c r="EB6" s="83"/>
+      <c r="EC6" s="83"/>
+      <c r="ED6" s="83"/>
+      <c r="EE6" s="83"/>
+      <c r="EF6" s="83"/>
+      <c r="EG6" s="83"/>
+      <c r="EH6" s="83"/>
+      <c r="EI6" s="83"/>
+      <c r="EJ6" s="83"/>
+      <c r="EK6" s="83"/>
+      <c r="EL6" s="83"/>
+      <c r="EM6" s="83"/>
+      <c r="EN6" s="83"/>
+      <c r="EO6" s="83"/>
+      <c r="EP6" s="83"/>
+      <c r="EQ6" s="83"/>
+      <c r="ER6" s="83"/>
+      <c r="ES6" s="83"/>
+      <c r="ET6" s="83"/>
+      <c r="EU6" s="83"/>
+      <c r="EV6" s="83"/>
+      <c r="EW6" s="83"/>
+      <c r="EX6" s="83"/>
+      <c r="EY6" s="83"/>
+      <c r="EZ6" s="83"/>
+      <c r="FA6" s="83"/>
+      <c r="FB6" s="83"/>
+      <c r="FC6" s="83"/>
+      <c r="FD6" s="83"/>
+      <c r="FE6" s="83"/>
+      <c r="FF6" s="83"/>
+      <c r="FG6" s="83"/>
+      <c r="FH6" s="83"/>
+      <c r="FI6" s="83"/>
+      <c r="FJ6" s="83"/>
+      <c r="FK6" s="83"/>
+      <c r="FL6" s="83"/>
+      <c r="FM6" s="83"/>
+      <c r="FN6" s="83"/>
+      <c r="FO6" s="83"/>
+      <c r="FP6" s="83"/>
+      <c r="FQ6" s="83"/>
+      <c r="FR6" s="83"/>
+      <c r="FS6" s="83"/>
+      <c r="FT6" s="83"/>
+      <c r="FU6" s="83"/>
+      <c r="FV6" s="83"/>
+      <c r="FW6" s="83"/>
+      <c r="FX6" s="83"/>
+      <c r="FY6" s="83"/>
+      <c r="FZ6" s="83"/>
+      <c r="GA6" s="83"/>
+      <c r="GB6" s="83"/>
+      <c r="GC6" s="83"/>
+      <c r="GD6" s="83"/>
+      <c r="GE6" s="83"/>
+      <c r="GF6" s="83"/>
+      <c r="GG6" s="83"/>
+      <c r="GH6" s="83"/>
+      <c r="GI6" s="83"/>
+      <c r="GJ6" s="83"/>
+      <c r="GK6" s="83"/>
+      <c r="GL6" s="83"/>
+      <c r="GM6" s="83"/>
+      <c r="GN6" s="83"/>
+      <c r="GO6" s="83"/>
+      <c r="GP6" s="83"/>
+      <c r="GQ6" s="83"/>
+      <c r="GR6" s="83"/>
+      <c r="GS6" s="83"/>
+      <c r="GT6" s="83"/>
+      <c r="GU6" s="83"/>
+      <c r="GV6" s="83"/>
+      <c r="GW6" s="83"/>
+      <c r="GX6" s="83"/>
+      <c r="GY6" s="83"/>
+      <c r="GZ6" s="83"/>
+      <c r="HA6" s="83"/>
+      <c r="HB6" s="83"/>
+      <c r="HC6" s="83"/>
+      <c r="HD6" s="83"/>
+      <c r="HE6" s="83"/>
+      <c r="HF6" s="83"/>
+      <c r="HG6" s="83"/>
+      <c r="HH6" s="83"/>
+      <c r="HI6" s="83"/>
+      <c r="HJ6" s="83"/>
+      <c r="HK6" s="83"/>
+      <c r="HL6" s="83"/>
+      <c r="HM6" s="83"/>
+      <c r="HN6" s="83"/>
+      <c r="HO6" s="83"/>
+      <c r="HP6" s="83"/>
+      <c r="HQ6" s="83"/>
+      <c r="HR6" s="83"/>
+      <c r="HS6" s="83"/>
+      <c r="HT6" s="83"/>
+      <c r="HU6" s="83"/>
+      <c r="HV6" s="83"/>
+      <c r="HW6" s="83"/>
+      <c r="HX6" s="83"/>
+      <c r="HY6" s="83"/>
+      <c r="HZ6" s="83"/>
+      <c r="IA6" s="83"/>
+      <c r="IB6" s="83"/>
+      <c r="IC6" s="83"/>
+      <c r="ID6" s="83"/>
+      <c r="IE6" s="83"/>
+      <c r="IF6" s="83"/>
     </row>
     <row r="7" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A7" s="98"/>
-      <c r="B7" s="107" t="s">
+      <c r="A7" s="85"/>
+      <c r="B7" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="95" t="s">
         <v>320</v>
       </c>
-      <c r="D7" s="108" t="s">
+      <c r="D7" s="95" t="s">
         <v>321</v>
       </c>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="108" t="s">
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="95" t="s">
         <v>322</v>
       </c>
-      <c r="J7" s="108"/>
-      <c r="K7" s="110">
+      <c r="J7" s="95"/>
+      <c r="K7" s="97">
         <v>2</v>
       </c>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="95" t="s">
         <v>323</v>
       </c>
-      <c r="M7" s="108" t="s">
+      <c r="M7" s="95" t="s">
         <v>324</v>
       </c>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="105"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="96"/>
-      <c r="V7" s="96"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="96"/>
-      <c r="Z7" s="96"/>
-      <c r="AA7" s="96"/>
-      <c r="AB7" s="96"/>
-      <c r="AC7" s="96"/>
-      <c r="AD7" s="96"/>
-      <c r="AE7" s="96"/>
-      <c r="AF7" s="96"/>
-      <c r="AG7" s="96"/>
-      <c r="AH7" s="96"/>
-      <c r="AI7" s="96"/>
-      <c r="AJ7" s="96"/>
-      <c r="AK7" s="96"/>
-      <c r="AL7" s="96"/>
-      <c r="AM7" s="96"/>
-      <c r="AN7" s="96"/>
-      <c r="AO7" s="96"/>
-      <c r="AP7" s="96"/>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="96"/>
-      <c r="AS7" s="96"/>
-      <c r="AT7" s="96"/>
-      <c r="AU7" s="96"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="AX7" s="96"/>
-      <c r="AY7" s="96"/>
-      <c r="AZ7" s="96"/>
-      <c r="BA7" s="96"/>
-      <c r="BB7" s="96"/>
-      <c r="BC7" s="96"/>
-      <c r="BD7" s="96"/>
-      <c r="BE7" s="96"/>
-      <c r="BF7" s="96"/>
-      <c r="BG7" s="96"/>
-      <c r="BH7" s="96"/>
-      <c r="BI7" s="96"/>
-      <c r="BJ7" s="96"/>
-      <c r="BK7" s="96"/>
-      <c r="BL7" s="96"/>
-      <c r="BM7" s="96"/>
-      <c r="BN7" s="96"/>
-      <c r="BO7" s="96"/>
-      <c r="BP7" s="96"/>
-      <c r="BQ7" s="96"/>
-      <c r="BR7" s="96"/>
-      <c r="BS7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BU7" s="96"/>
-      <c r="BV7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="BX7" s="96"/>
-      <c r="BY7" s="96"/>
-      <c r="BZ7" s="96"/>
-      <c r="CA7" s="96"/>
-      <c r="CB7" s="96"/>
-      <c r="CC7" s="96"/>
-      <c r="CD7" s="96"/>
-      <c r="CE7" s="96"/>
-      <c r="CF7" s="96"/>
-      <c r="CG7" s="96"/>
-      <c r="CH7" s="96"/>
-      <c r="CI7" s="96"/>
-      <c r="CJ7" s="96"/>
-      <c r="CK7" s="96"/>
-      <c r="CL7" s="96"/>
-      <c r="CM7" s="96"/>
-      <c r="CN7" s="96"/>
-      <c r="CO7" s="96"/>
-      <c r="CP7" s="96"/>
-      <c r="CQ7" s="96"/>
-      <c r="CR7" s="96"/>
-      <c r="CS7" s="96"/>
-      <c r="CT7" s="96"/>
-      <c r="CU7" s="96"/>
-      <c r="CV7" s="96"/>
-      <c r="CW7" s="96"/>
-      <c r="CX7" s="96"/>
-      <c r="CY7" s="96"/>
-      <c r="CZ7" s="96"/>
-      <c r="DA7" s="96"/>
-      <c r="DB7" s="96"/>
-      <c r="DC7" s="96"/>
-      <c r="DD7" s="96"/>
-      <c r="DE7" s="96"/>
-      <c r="DF7" s="96"/>
-      <c r="DG7" s="96"/>
-      <c r="DH7" s="96"/>
-      <c r="DI7" s="96"/>
-      <c r="DJ7" s="96"/>
-      <c r="DK7" s="96"/>
-      <c r="DL7" s="96"/>
-      <c r="DM7" s="96"/>
-      <c r="DN7" s="96"/>
-      <c r="DO7" s="96"/>
-      <c r="DP7" s="96"/>
-      <c r="DQ7" s="96"/>
-      <c r="DR7" s="96"/>
-      <c r="DS7" s="96"/>
-      <c r="DT7" s="96"/>
-      <c r="DU7" s="96"/>
-      <c r="DV7" s="96"/>
-      <c r="DW7" s="96"/>
-      <c r="DX7" s="96"/>
-      <c r="DY7" s="96"/>
-      <c r="DZ7" s="96"/>
-      <c r="EA7" s="96"/>
-      <c r="EB7" s="96"/>
-      <c r="EC7" s="96"/>
-      <c r="ED7" s="96"/>
-      <c r="EE7" s="96"/>
-      <c r="EF7" s="96"/>
-      <c r="EG7" s="96"/>
-      <c r="EH7" s="96"/>
-      <c r="EI7" s="96"/>
-      <c r="EJ7" s="96"/>
-      <c r="EK7" s="96"/>
-      <c r="EL7" s="96"/>
-      <c r="EM7" s="96"/>
-      <c r="EN7" s="96"/>
-      <c r="EO7" s="96"/>
-      <c r="EP7" s="96"/>
-      <c r="EQ7" s="96"/>
-      <c r="ER7" s="96"/>
-      <c r="ES7" s="96"/>
-      <c r="ET7" s="96"/>
-      <c r="EU7" s="96"/>
-      <c r="EV7" s="96"/>
-      <c r="EW7" s="96"/>
-      <c r="EX7" s="96"/>
-      <c r="EY7" s="96"/>
-      <c r="EZ7" s="96"/>
-      <c r="FA7" s="96"/>
-      <c r="FB7" s="96"/>
-      <c r="FC7" s="96"/>
-      <c r="FD7" s="96"/>
-      <c r="FE7" s="96"/>
-      <c r="FF7" s="96"/>
-      <c r="FG7" s="96"/>
-      <c r="FH7" s="96"/>
-      <c r="FI7" s="96"/>
-      <c r="FJ7" s="96"/>
-      <c r="FK7" s="96"/>
-      <c r="FL7" s="96"/>
-      <c r="FM7" s="96"/>
-      <c r="FN7" s="96"/>
-      <c r="FO7" s="96"/>
-      <c r="FP7" s="96"/>
-      <c r="FQ7" s="96"/>
-      <c r="FR7" s="96"/>
-      <c r="FS7" s="96"/>
-      <c r="FT7" s="96"/>
-      <c r="FU7" s="96"/>
-      <c r="FV7" s="96"/>
-      <c r="FW7" s="96"/>
-      <c r="FX7" s="96"/>
-      <c r="FY7" s="96"/>
-      <c r="FZ7" s="96"/>
-      <c r="GA7" s="96"/>
-      <c r="GB7" s="96"/>
-      <c r="GC7" s="96"/>
-      <c r="GD7" s="96"/>
-      <c r="GE7" s="96"/>
-      <c r="GF7" s="96"/>
-      <c r="GG7" s="96"/>
-      <c r="GH7" s="96"/>
-      <c r="GI7" s="96"/>
-      <c r="GJ7" s="96"/>
-      <c r="GK7" s="96"/>
-      <c r="GL7" s="96"/>
-      <c r="GM7" s="96"/>
-      <c r="GN7" s="96"/>
-      <c r="GO7" s="96"/>
-      <c r="GP7" s="96"/>
-      <c r="GQ7" s="96"/>
-      <c r="GR7" s="96"/>
-      <c r="GS7" s="96"/>
-      <c r="GT7" s="96"/>
-      <c r="GU7" s="96"/>
-      <c r="GV7" s="96"/>
-      <c r="GW7" s="96"/>
-      <c r="GX7" s="96"/>
-      <c r="GY7" s="96"/>
-      <c r="GZ7" s="96"/>
-      <c r="HA7" s="96"/>
-      <c r="HB7" s="96"/>
-      <c r="HC7" s="96"/>
-      <c r="HD7" s="96"/>
-      <c r="HE7" s="96"/>
-      <c r="HF7" s="96"/>
-      <c r="HG7" s="96"/>
-      <c r="HH7" s="96"/>
-      <c r="HI7" s="96"/>
-      <c r="HJ7" s="96"/>
-      <c r="HK7" s="96"/>
-      <c r="HL7" s="96"/>
-      <c r="HM7" s="96"/>
-      <c r="HN7" s="96"/>
-      <c r="HO7" s="96"/>
-      <c r="HP7" s="96"/>
-      <c r="HQ7" s="96"/>
-      <c r="HR7" s="96"/>
-      <c r="HS7" s="96"/>
-      <c r="HT7" s="96"/>
-      <c r="HU7" s="96"/>
-      <c r="HV7" s="96"/>
-      <c r="HW7" s="96"/>
-      <c r="HX7" s="96"/>
-      <c r="HY7" s="96"/>
-      <c r="HZ7" s="96"/>
-      <c r="IA7" s="96"/>
-      <c r="IB7" s="96"/>
-      <c r="IC7" s="96"/>
-      <c r="ID7" s="96"/>
-      <c r="IE7" s="96"/>
-      <c r="IF7" s="96"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="84"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="83"/>
+      <c r="AJ7" s="83"/>
+      <c r="AK7" s="83"/>
+      <c r="AL7" s="83"/>
+      <c r="AM7" s="83"/>
+      <c r="AN7" s="83"/>
+      <c r="AO7" s="83"/>
+      <c r="AP7" s="83"/>
+      <c r="AQ7" s="83"/>
+      <c r="AR7" s="83"/>
+      <c r="AS7" s="83"/>
+      <c r="AT7" s="83"/>
+      <c r="AU7" s="83"/>
+      <c r="AV7" s="83"/>
+      <c r="AW7" s="83"/>
+      <c r="AX7" s="83"/>
+      <c r="AY7" s="83"/>
+      <c r="AZ7" s="83"/>
+      <c r="BA7" s="83"/>
+      <c r="BB7" s="83"/>
+      <c r="BC7" s="83"/>
+      <c r="BD7" s="83"/>
+      <c r="BE7" s="83"/>
+      <c r="BF7" s="83"/>
+      <c r="BG7" s="83"/>
+      <c r="BH7" s="83"/>
+      <c r="BI7" s="83"/>
+      <c r="BJ7" s="83"/>
+      <c r="BK7" s="83"/>
+      <c r="BL7" s="83"/>
+      <c r="BM7" s="83"/>
+      <c r="BN7" s="83"/>
+      <c r="BO7" s="83"/>
+      <c r="BP7" s="83"/>
+      <c r="BQ7" s="83"/>
+      <c r="BR7" s="83"/>
+      <c r="BS7" s="83"/>
+      <c r="BT7" s="83"/>
+      <c r="BU7" s="83"/>
+      <c r="BV7" s="83"/>
+      <c r="BW7" s="83"/>
+      <c r="BX7" s="83"/>
+      <c r="BY7" s="83"/>
+      <c r="BZ7" s="83"/>
+      <c r="CA7" s="83"/>
+      <c r="CB7" s="83"/>
+      <c r="CC7" s="83"/>
+      <c r="CD7" s="83"/>
+      <c r="CE7" s="83"/>
+      <c r="CF7" s="83"/>
+      <c r="CG7" s="83"/>
+      <c r="CH7" s="83"/>
+      <c r="CI7" s="83"/>
+      <c r="CJ7" s="83"/>
+      <c r="CK7" s="83"/>
+      <c r="CL7" s="83"/>
+      <c r="CM7" s="83"/>
+      <c r="CN7" s="83"/>
+      <c r="CO7" s="83"/>
+      <c r="CP7" s="83"/>
+      <c r="CQ7" s="83"/>
+      <c r="CR7" s="83"/>
+      <c r="CS7" s="83"/>
+      <c r="CT7" s="83"/>
+      <c r="CU7" s="83"/>
+      <c r="CV7" s="83"/>
+      <c r="CW7" s="83"/>
+      <c r="CX7" s="83"/>
+      <c r="CY7" s="83"/>
+      <c r="CZ7" s="83"/>
+      <c r="DA7" s="83"/>
+      <c r="DB7" s="83"/>
+      <c r="DC7" s="83"/>
+      <c r="DD7" s="83"/>
+      <c r="DE7" s="83"/>
+      <c r="DF7" s="83"/>
+      <c r="DG7" s="83"/>
+      <c r="DH7" s="83"/>
+      <c r="DI7" s="83"/>
+      <c r="DJ7" s="83"/>
+      <c r="DK7" s="83"/>
+      <c r="DL7" s="83"/>
+      <c r="DM7" s="83"/>
+      <c r="DN7" s="83"/>
+      <c r="DO7" s="83"/>
+      <c r="DP7" s="83"/>
+      <c r="DQ7" s="83"/>
+      <c r="DR7" s="83"/>
+      <c r="DS7" s="83"/>
+      <c r="DT7" s="83"/>
+      <c r="DU7" s="83"/>
+      <c r="DV7" s="83"/>
+      <c r="DW7" s="83"/>
+      <c r="DX7" s="83"/>
+      <c r="DY7" s="83"/>
+      <c r="DZ7" s="83"/>
+      <c r="EA7" s="83"/>
+      <c r="EB7" s="83"/>
+      <c r="EC7" s="83"/>
+      <c r="ED7" s="83"/>
+      <c r="EE7" s="83"/>
+      <c r="EF7" s="83"/>
+      <c r="EG7" s="83"/>
+      <c r="EH7" s="83"/>
+      <c r="EI7" s="83"/>
+      <c r="EJ7" s="83"/>
+      <c r="EK7" s="83"/>
+      <c r="EL7" s="83"/>
+      <c r="EM7" s="83"/>
+      <c r="EN7" s="83"/>
+      <c r="EO7" s="83"/>
+      <c r="EP7" s="83"/>
+      <c r="EQ7" s="83"/>
+      <c r="ER7" s="83"/>
+      <c r="ES7" s="83"/>
+      <c r="ET7" s="83"/>
+      <c r="EU7" s="83"/>
+      <c r="EV7" s="83"/>
+      <c r="EW7" s="83"/>
+      <c r="EX7" s="83"/>
+      <c r="EY7" s="83"/>
+      <c r="EZ7" s="83"/>
+      <c r="FA7" s="83"/>
+      <c r="FB7" s="83"/>
+      <c r="FC7" s="83"/>
+      <c r="FD7" s="83"/>
+      <c r="FE7" s="83"/>
+      <c r="FF7" s="83"/>
+      <c r="FG7" s="83"/>
+      <c r="FH7" s="83"/>
+      <c r="FI7" s="83"/>
+      <c r="FJ7" s="83"/>
+      <c r="FK7" s="83"/>
+      <c r="FL7" s="83"/>
+      <c r="FM7" s="83"/>
+      <c r="FN7" s="83"/>
+      <c r="FO7" s="83"/>
+      <c r="FP7" s="83"/>
+      <c r="FQ7" s="83"/>
+      <c r="FR7" s="83"/>
+      <c r="FS7" s="83"/>
+      <c r="FT7" s="83"/>
+      <c r="FU7" s="83"/>
+      <c r="FV7" s="83"/>
+      <c r="FW7" s="83"/>
+      <c r="FX7" s="83"/>
+      <c r="FY7" s="83"/>
+      <c r="FZ7" s="83"/>
+      <c r="GA7" s="83"/>
+      <c r="GB7" s="83"/>
+      <c r="GC7" s="83"/>
+      <c r="GD7" s="83"/>
+      <c r="GE7" s="83"/>
+      <c r="GF7" s="83"/>
+      <c r="GG7" s="83"/>
+      <c r="GH7" s="83"/>
+      <c r="GI7" s="83"/>
+      <c r="GJ7" s="83"/>
+      <c r="GK7" s="83"/>
+      <c r="GL7" s="83"/>
+      <c r="GM7" s="83"/>
+      <c r="GN7" s="83"/>
+      <c r="GO7" s="83"/>
+      <c r="GP7" s="83"/>
+      <c r="GQ7" s="83"/>
+      <c r="GR7" s="83"/>
+      <c r="GS7" s="83"/>
+      <c r="GT7" s="83"/>
+      <c r="GU7" s="83"/>
+      <c r="GV7" s="83"/>
+      <c r="GW7" s="83"/>
+      <c r="GX7" s="83"/>
+      <c r="GY7" s="83"/>
+      <c r="GZ7" s="83"/>
+      <c r="HA7" s="83"/>
+      <c r="HB7" s="83"/>
+      <c r="HC7" s="83"/>
+      <c r="HD7" s="83"/>
+      <c r="HE7" s="83"/>
+      <c r="HF7" s="83"/>
+      <c r="HG7" s="83"/>
+      <c r="HH7" s="83"/>
+      <c r="HI7" s="83"/>
+      <c r="HJ7" s="83"/>
+      <c r="HK7" s="83"/>
+      <c r="HL7" s="83"/>
+      <c r="HM7" s="83"/>
+      <c r="HN7" s="83"/>
+      <c r="HO7" s="83"/>
+      <c r="HP7" s="83"/>
+      <c r="HQ7" s="83"/>
+      <c r="HR7" s="83"/>
+      <c r="HS7" s="83"/>
+      <c r="HT7" s="83"/>
+      <c r="HU7" s="83"/>
+      <c r="HV7" s="83"/>
+      <c r="HW7" s="83"/>
+      <c r="HX7" s="83"/>
+      <c r="HY7" s="83"/>
+      <c r="HZ7" s="83"/>
+      <c r="IA7" s="83"/>
+      <c r="IB7" s="83"/>
+      <c r="IC7" s="83"/>
+      <c r="ID7" s="83"/>
+      <c r="IE7" s="83"/>
+      <c r="IF7" s="83"/>
     </row>
     <row r="8" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A8" s="98"/>
-      <c r="B8" s="107" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="94" t="s">
         <v>325</v>
       </c>
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="95" t="s">
         <v>326</v>
       </c>
-      <c r="D8" s="108" t="s">
+      <c r="D8" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="108" t="s">
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="95" t="s">
         <v>322</v>
       </c>
-      <c r="J8" s="108"/>
-      <c r="K8" s="110">
+      <c r="J8" s="95"/>
+      <c r="K8" s="97">
         <v>1</v>
       </c>
-      <c r="L8" s="108" t="s">
+      <c r="L8" s="95" t="s">
         <v>327</v>
       </c>
-      <c r="M8" s="108" t="s">
+      <c r="M8" s="95" t="s">
         <v>328</v>
       </c>
-      <c r="N8" s="97"/>
-      <c r="O8" s="97"/>
-      <c r="P8" s="105"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="96"/>
-      <c r="U8" s="96"/>
-      <c r="V8" s="96"/>
-      <c r="W8" s="96"/>
-      <c r="X8" s="96"/>
-      <c r="Y8" s="96"/>
-      <c r="Z8" s="96"/>
-      <c r="AA8" s="96"/>
-      <c r="AB8" s="96"/>
-      <c r="AC8" s="96"/>
-      <c r="AD8" s="96"/>
-      <c r="AE8" s="96"/>
-      <c r="AF8" s="96"/>
-      <c r="AG8" s="96"/>
-      <c r="AH8" s="96"/>
-      <c r="AI8" s="96"/>
-      <c r="AJ8" s="96"/>
-      <c r="AK8" s="96"/>
-      <c r="AL8" s="96"/>
-      <c r="AM8" s="96"/>
-      <c r="AN8" s="96"/>
-      <c r="AO8" s="96"/>
-      <c r="AP8" s="96"/>
-      <c r="AQ8" s="96"/>
-      <c r="AR8" s="96"/>
-      <c r="AS8" s="96"/>
-      <c r="AT8" s="96"/>
-      <c r="AU8" s="96"/>
-      <c r="AV8" s="96"/>
-      <c r="AW8" s="96"/>
-      <c r="AX8" s="96"/>
-      <c r="AY8" s="96"/>
-      <c r="AZ8" s="96"/>
-      <c r="BA8" s="96"/>
-      <c r="BB8" s="96"/>
-      <c r="BC8" s="96"/>
-      <c r="BD8" s="96"/>
-      <c r="BE8" s="96"/>
-      <c r="BF8" s="96"/>
-      <c r="BG8" s="96"/>
-      <c r="BH8" s="96"/>
-      <c r="BI8" s="96"/>
-      <c r="BJ8" s="96"/>
-      <c r="BK8" s="96"/>
-      <c r="BL8" s="96"/>
-      <c r="BM8" s="96"/>
-      <c r="BN8" s="96"/>
-      <c r="BO8" s="96"/>
-      <c r="BP8" s="96"/>
-      <c r="BQ8" s="96"/>
-      <c r="BR8" s="96"/>
-      <c r="BS8" s="96"/>
-      <c r="BT8" s="96"/>
-      <c r="BU8" s="96"/>
-      <c r="BV8" s="96"/>
-      <c r="BW8" s="96"/>
-      <c r="BX8" s="96"/>
-      <c r="BY8" s="96"/>
-      <c r="BZ8" s="96"/>
-      <c r="CA8" s="96"/>
-      <c r="CB8" s="96"/>
-      <c r="CC8" s="96"/>
-      <c r="CD8" s="96"/>
-      <c r="CE8" s="96"/>
-      <c r="CF8" s="96"/>
-      <c r="CG8" s="96"/>
-      <c r="CH8" s="96"/>
-      <c r="CI8" s="96"/>
-      <c r="CJ8" s="96"/>
-      <c r="CK8" s="96"/>
-      <c r="CL8" s="96"/>
-      <c r="CM8" s="96"/>
-      <c r="CN8" s="96"/>
-      <c r="CO8" s="96"/>
-      <c r="CP8" s="96"/>
-      <c r="CQ8" s="96"/>
-      <c r="CR8" s="96"/>
-      <c r="CS8" s="96"/>
-      <c r="CT8" s="96"/>
-      <c r="CU8" s="96"/>
-      <c r="CV8" s="96"/>
-      <c r="CW8" s="96"/>
-      <c r="CX8" s="96"/>
-      <c r="CY8" s="96"/>
-      <c r="CZ8" s="96"/>
-      <c r="DA8" s="96"/>
-      <c r="DB8" s="96"/>
-      <c r="DC8" s="96"/>
-      <c r="DD8" s="96"/>
-      <c r="DE8" s="96"/>
-      <c r="DF8" s="96"/>
-      <c r="DG8" s="96"/>
-      <c r="DH8" s="96"/>
-      <c r="DI8" s="96"/>
-      <c r="DJ8" s="96"/>
-      <c r="DK8" s="96"/>
-      <c r="DL8" s="96"/>
-      <c r="DM8" s="96"/>
-      <c r="DN8" s="96"/>
-      <c r="DO8" s="96"/>
-      <c r="DP8" s="96"/>
-      <c r="DQ8" s="96"/>
-      <c r="DR8" s="96"/>
-      <c r="DS8" s="96"/>
-      <c r="DT8" s="96"/>
-      <c r="DU8" s="96"/>
-      <c r="DV8" s="96"/>
-      <c r="DW8" s="96"/>
-      <c r="DX8" s="96"/>
-      <c r="DY8" s="96"/>
-      <c r="DZ8" s="96"/>
-      <c r="EA8" s="96"/>
-      <c r="EB8" s="96"/>
-      <c r="EC8" s="96"/>
-      <c r="ED8" s="96"/>
-      <c r="EE8" s="96"/>
-      <c r="EF8" s="96"/>
-      <c r="EG8" s="96"/>
-      <c r="EH8" s="96"/>
-      <c r="EI8" s="96"/>
-      <c r="EJ8" s="96"/>
-      <c r="EK8" s="96"/>
-      <c r="EL8" s="96"/>
-      <c r="EM8" s="96"/>
-      <c r="EN8" s="96"/>
-      <c r="EO8" s="96"/>
-      <c r="EP8" s="96"/>
-      <c r="EQ8" s="96"/>
-      <c r="ER8" s="96"/>
-      <c r="ES8" s="96"/>
-      <c r="ET8" s="96"/>
-      <c r="EU8" s="96"/>
-      <c r="EV8" s="96"/>
-      <c r="EW8" s="96"/>
-      <c r="EX8" s="96"/>
-      <c r="EY8" s="96"/>
-      <c r="EZ8" s="96"/>
-      <c r="FA8" s="96"/>
-      <c r="FB8" s="96"/>
-      <c r="FC8" s="96"/>
-      <c r="FD8" s="96"/>
-      <c r="FE8" s="96"/>
-      <c r="FF8" s="96"/>
-      <c r="FG8" s="96"/>
-      <c r="FH8" s="96"/>
-      <c r="FI8" s="96"/>
-      <c r="FJ8" s="96"/>
-      <c r="FK8" s="96"/>
-      <c r="FL8" s="96"/>
-      <c r="FM8" s="96"/>
-      <c r="FN8" s="96"/>
-      <c r="FO8" s="96"/>
-      <c r="FP8" s="96"/>
-      <c r="FQ8" s="96"/>
-      <c r="FR8" s="96"/>
-      <c r="FS8" s="96"/>
-      <c r="FT8" s="96"/>
-      <c r="FU8" s="96"/>
-      <c r="FV8" s="96"/>
-      <c r="FW8" s="96"/>
-      <c r="FX8" s="96"/>
-      <c r="FY8" s="96"/>
-      <c r="FZ8" s="96"/>
-      <c r="GA8" s="96"/>
-      <c r="GB8" s="96"/>
-      <c r="GC8" s="96"/>
-      <c r="GD8" s="96"/>
-      <c r="GE8" s="96"/>
-      <c r="GF8" s="96"/>
-      <c r="GG8" s="96"/>
-      <c r="GH8" s="96"/>
-      <c r="GI8" s="96"/>
-      <c r="GJ8" s="96"/>
-      <c r="GK8" s="96"/>
-      <c r="GL8" s="96"/>
-      <c r="GM8" s="96"/>
-      <c r="GN8" s="96"/>
-      <c r="GO8" s="96"/>
-      <c r="GP8" s="96"/>
-      <c r="GQ8" s="96"/>
-      <c r="GR8" s="96"/>
-      <c r="GS8" s="96"/>
-      <c r="GT8" s="96"/>
-      <c r="GU8" s="96"/>
-      <c r="GV8" s="96"/>
-      <c r="GW8" s="96"/>
-      <c r="GX8" s="96"/>
-      <c r="GY8" s="96"/>
-      <c r="GZ8" s="96"/>
-      <c r="HA8" s="96"/>
-      <c r="HB8" s="96"/>
-      <c r="HC8" s="96"/>
-      <c r="HD8" s="96"/>
-      <c r="HE8" s="96"/>
-      <c r="HF8" s="96"/>
-      <c r="HG8" s="96"/>
-      <c r="HH8" s="96"/>
-      <c r="HI8" s="96"/>
-      <c r="HJ8" s="96"/>
-      <c r="HK8" s="96"/>
-      <c r="HL8" s="96"/>
-      <c r="HM8" s="96"/>
-      <c r="HN8" s="96"/>
-      <c r="HO8" s="96"/>
-      <c r="HP8" s="96"/>
-      <c r="HQ8" s="96"/>
-      <c r="HR8" s="96"/>
-      <c r="HS8" s="96"/>
-      <c r="HT8" s="96"/>
-      <c r="HU8" s="96"/>
-      <c r="HV8" s="96"/>
-      <c r="HW8" s="96"/>
-      <c r="HX8" s="96"/>
-      <c r="HY8" s="96"/>
-      <c r="HZ8" s="96"/>
-      <c r="IA8" s="96"/>
-      <c r="IB8" s="96"/>
-      <c r="IC8" s="96"/>
-      <c r="ID8" s="96"/>
-      <c r="IE8" s="96"/>
-      <c r="IF8" s="96"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="84"/>
+      <c r="P8" s="92"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="83"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="83"/>
+      <c r="AB8" s="83"/>
+      <c r="AC8" s="83"/>
+      <c r="AD8" s="83"/>
+      <c r="AE8" s="83"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="83"/>
+      <c r="AH8" s="83"/>
+      <c r="AI8" s="83"/>
+      <c r="AJ8" s="83"/>
+      <c r="AK8" s="83"/>
+      <c r="AL8" s="83"/>
+      <c r="AM8" s="83"/>
+      <c r="AN8" s="83"/>
+      <c r="AO8" s="83"/>
+      <c r="AP8" s="83"/>
+      <c r="AQ8" s="83"/>
+      <c r="AR8" s="83"/>
+      <c r="AS8" s="83"/>
+      <c r="AT8" s="83"/>
+      <c r="AU8" s="83"/>
+      <c r="AV8" s="83"/>
+      <c r="AW8" s="83"/>
+      <c r="AX8" s="83"/>
+      <c r="AY8" s="83"/>
+      <c r="AZ8" s="83"/>
+      <c r="BA8" s="83"/>
+      <c r="BB8" s="83"/>
+      <c r="BC8" s="83"/>
+      <c r="BD8" s="83"/>
+      <c r="BE8" s="83"/>
+      <c r="BF8" s="83"/>
+      <c r="BG8" s="83"/>
+      <c r="BH8" s="83"/>
+      <c r="BI8" s="83"/>
+      <c r="BJ8" s="83"/>
+      <c r="BK8" s="83"/>
+      <c r="BL8" s="83"/>
+      <c r="BM8" s="83"/>
+      <c r="BN8" s="83"/>
+      <c r="BO8" s="83"/>
+      <c r="BP8" s="83"/>
+      <c r="BQ8" s="83"/>
+      <c r="BR8" s="83"/>
+      <c r="BS8" s="83"/>
+      <c r="BT8" s="83"/>
+      <c r="BU8" s="83"/>
+      <c r="BV8" s="83"/>
+      <c r="BW8" s="83"/>
+      <c r="BX8" s="83"/>
+      <c r="BY8" s="83"/>
+      <c r="BZ8" s="83"/>
+      <c r="CA8" s="83"/>
+      <c r="CB8" s="83"/>
+      <c r="CC8" s="83"/>
+      <c r="CD8" s="83"/>
+      <c r="CE8" s="83"/>
+      <c r="CF8" s="83"/>
+      <c r="CG8" s="83"/>
+      <c r="CH8" s="83"/>
+      <c r="CI8" s="83"/>
+      <c r="CJ8" s="83"/>
+      <c r="CK8" s="83"/>
+      <c r="CL8" s="83"/>
+      <c r="CM8" s="83"/>
+      <c r="CN8" s="83"/>
+      <c r="CO8" s="83"/>
+      <c r="CP8" s="83"/>
+      <c r="CQ8" s="83"/>
+      <c r="CR8" s="83"/>
+      <c r="CS8" s="83"/>
+      <c r="CT8" s="83"/>
+      <c r="CU8" s="83"/>
+      <c r="CV8" s="83"/>
+      <c r="CW8" s="83"/>
+      <c r="CX8" s="83"/>
+      <c r="CY8" s="83"/>
+      <c r="CZ8" s="83"/>
+      <c r="DA8" s="83"/>
+      <c r="DB8" s="83"/>
+      <c r="DC8" s="83"/>
+      <c r="DD8" s="83"/>
+      <c r="DE8" s="83"/>
+      <c r="DF8" s="83"/>
+      <c r="DG8" s="83"/>
+      <c r="DH8" s="83"/>
+      <c r="DI8" s="83"/>
+      <c r="DJ8" s="83"/>
+      <c r="DK8" s="83"/>
+      <c r="DL8" s="83"/>
+      <c r="DM8" s="83"/>
+      <c r="DN8" s="83"/>
+      <c r="DO8" s="83"/>
+      <c r="DP8" s="83"/>
+      <c r="DQ8" s="83"/>
+      <c r="DR8" s="83"/>
+      <c r="DS8" s="83"/>
+      <c r="DT8" s="83"/>
+      <c r="DU8" s="83"/>
+      <c r="DV8" s="83"/>
+      <c r="DW8" s="83"/>
+      <c r="DX8" s="83"/>
+      <c r="DY8" s="83"/>
+      <c r="DZ8" s="83"/>
+      <c r="EA8" s="83"/>
+      <c r="EB8" s="83"/>
+      <c r="EC8" s="83"/>
+      <c r="ED8" s="83"/>
+      <c r="EE8" s="83"/>
+      <c r="EF8" s="83"/>
+      <c r="EG8" s="83"/>
+      <c r="EH8" s="83"/>
+      <c r="EI8" s="83"/>
+      <c r="EJ8" s="83"/>
+      <c r="EK8" s="83"/>
+      <c r="EL8" s="83"/>
+      <c r="EM8" s="83"/>
+      <c r="EN8" s="83"/>
+      <c r="EO8" s="83"/>
+      <c r="EP8" s="83"/>
+      <c r="EQ8" s="83"/>
+      <c r="ER8" s="83"/>
+      <c r="ES8" s="83"/>
+      <c r="ET8" s="83"/>
+      <c r="EU8" s="83"/>
+      <c r="EV8" s="83"/>
+      <c r="EW8" s="83"/>
+      <c r="EX8" s="83"/>
+      <c r="EY8" s="83"/>
+      <c r="EZ8" s="83"/>
+      <c r="FA8" s="83"/>
+      <c r="FB8" s="83"/>
+      <c r="FC8" s="83"/>
+      <c r="FD8" s="83"/>
+      <c r="FE8" s="83"/>
+      <c r="FF8" s="83"/>
+      <c r="FG8" s="83"/>
+      <c r="FH8" s="83"/>
+      <c r="FI8" s="83"/>
+      <c r="FJ8" s="83"/>
+      <c r="FK8" s="83"/>
+      <c r="FL8" s="83"/>
+      <c r="FM8" s="83"/>
+      <c r="FN8" s="83"/>
+      <c r="FO8" s="83"/>
+      <c r="FP8" s="83"/>
+      <c r="FQ8" s="83"/>
+      <c r="FR8" s="83"/>
+      <c r="FS8" s="83"/>
+      <c r="FT8" s="83"/>
+      <c r="FU8" s="83"/>
+      <c r="FV8" s="83"/>
+      <c r="FW8" s="83"/>
+      <c r="FX8" s="83"/>
+      <c r="FY8" s="83"/>
+      <c r="FZ8" s="83"/>
+      <c r="GA8" s="83"/>
+      <c r="GB8" s="83"/>
+      <c r="GC8" s="83"/>
+      <c r="GD8" s="83"/>
+      <c r="GE8" s="83"/>
+      <c r="GF8" s="83"/>
+      <c r="GG8" s="83"/>
+      <c r="GH8" s="83"/>
+      <c r="GI8" s="83"/>
+      <c r="GJ8" s="83"/>
+      <c r="GK8" s="83"/>
+      <c r="GL8" s="83"/>
+      <c r="GM8" s="83"/>
+      <c r="GN8" s="83"/>
+      <c r="GO8" s="83"/>
+      <c r="GP8" s="83"/>
+      <c r="GQ8" s="83"/>
+      <c r="GR8" s="83"/>
+      <c r="GS8" s="83"/>
+      <c r="GT8" s="83"/>
+      <c r="GU8" s="83"/>
+      <c r="GV8" s="83"/>
+      <c r="GW8" s="83"/>
+      <c r="GX8" s="83"/>
+      <c r="GY8" s="83"/>
+      <c r="GZ8" s="83"/>
+      <c r="HA8" s="83"/>
+      <c r="HB8" s="83"/>
+      <c r="HC8" s="83"/>
+      <c r="HD8" s="83"/>
+      <c r="HE8" s="83"/>
+      <c r="HF8" s="83"/>
+      <c r="HG8" s="83"/>
+      <c r="HH8" s="83"/>
+      <c r="HI8" s="83"/>
+      <c r="HJ8" s="83"/>
+      <c r="HK8" s="83"/>
+      <c r="HL8" s="83"/>
+      <c r="HM8" s="83"/>
+      <c r="HN8" s="83"/>
+      <c r="HO8" s="83"/>
+      <c r="HP8" s="83"/>
+      <c r="HQ8" s="83"/>
+      <c r="HR8" s="83"/>
+      <c r="HS8" s="83"/>
+      <c r="HT8" s="83"/>
+      <c r="HU8" s="83"/>
+      <c r="HV8" s="83"/>
+      <c r="HW8" s="83"/>
+      <c r="HX8" s="83"/>
+      <c r="HY8" s="83"/>
+      <c r="HZ8" s="83"/>
+      <c r="IA8" s="83"/>
+      <c r="IB8" s="83"/>
+      <c r="IC8" s="83"/>
+      <c r="ID8" s="83"/>
+      <c r="IE8" s="83"/>
+      <c r="IF8" s="83"/>
     </row>
     <row r="9" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A9" s="98"/>
-      <c r="B9" s="107" t="s">
+      <c r="A9" s="85"/>
+      <c r="B9" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="95" t="s">
         <v>329</v>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="108" t="s">
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="95" t="s">
         <v>330</v>
       </c>
-      <c r="J9" s="108"/>
-      <c r="K9" s="110">
+      <c r="J9" s="95"/>
+      <c r="K9" s="97">
         <v>1</v>
       </c>
-      <c r="L9" s="108" t="s">
+      <c r="L9" s="95" t="s">
         <v>340</v>
       </c>
-      <c r="M9" s="108" t="s">
+      <c r="M9" s="95" t="s">
         <v>331</v>
       </c>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="106"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="96"/>
-      <c r="U9" s="96"/>
-      <c r="V9" s="96"/>
-      <c r="W9" s="96"/>
-      <c r="X9" s="96"/>
-      <c r="Y9" s="96"/>
-      <c r="Z9" s="96"/>
-      <c r="AA9" s="96"/>
-      <c r="AB9" s="96"/>
-      <c r="AC9" s="96"/>
-      <c r="AD9" s="96"/>
-      <c r="AE9" s="96"/>
-      <c r="AF9" s="96"/>
-      <c r="AG9" s="96"/>
-      <c r="AH9" s="96"/>
-      <c r="AI9" s="96"/>
-      <c r="AJ9" s="96"/>
-      <c r="AK9" s="96"/>
-      <c r="AL9" s="96"/>
-      <c r="AM9" s="96"/>
-      <c r="AN9" s="96"/>
-      <c r="AO9" s="96"/>
-      <c r="AP9" s="96"/>
-      <c r="AQ9" s="96"/>
-      <c r="AR9" s="96"/>
-      <c r="AS9" s="96"/>
-      <c r="AT9" s="96"/>
-      <c r="AU9" s="96"/>
-      <c r="AV9" s="96"/>
-      <c r="AW9" s="96"/>
-      <c r="AX9" s="96"/>
-      <c r="AY9" s="96"/>
-      <c r="AZ9" s="96"/>
-      <c r="BA9" s="96"/>
-      <c r="BB9" s="96"/>
-      <c r="BC9" s="96"/>
-      <c r="BD9" s="96"/>
-      <c r="BE9" s="96"/>
-      <c r="BF9" s="96"/>
-      <c r="BG9" s="96"/>
-      <c r="BH9" s="96"/>
-      <c r="BI9" s="96"/>
-      <c r="BJ9" s="96"/>
-      <c r="BK9" s="96"/>
-      <c r="BL9" s="96"/>
-      <c r="BM9" s="96"/>
-      <c r="BN9" s="96"/>
-      <c r="BO9" s="96"/>
-      <c r="BP9" s="96"/>
-      <c r="BQ9" s="96"/>
-      <c r="BR9" s="96"/>
-      <c r="BS9" s="96"/>
-      <c r="BT9" s="96"/>
-      <c r="BU9" s="96"/>
-      <c r="BV9" s="96"/>
-      <c r="BW9" s="96"/>
-      <c r="BX9" s="96"/>
-      <c r="BY9" s="96"/>
-      <c r="BZ9" s="96"/>
-      <c r="CA9" s="96"/>
-      <c r="CB9" s="96"/>
-      <c r="CC9" s="96"/>
-      <c r="CD9" s="96"/>
-      <c r="CE9" s="96"/>
-      <c r="CF9" s="96"/>
-      <c r="CG9" s="96"/>
-      <c r="CH9" s="96"/>
-      <c r="CI9" s="96"/>
-      <c r="CJ9" s="96"/>
-      <c r="CK9" s="96"/>
-      <c r="CL9" s="96"/>
-      <c r="CM9" s="96"/>
-      <c r="CN9" s="96"/>
-      <c r="CO9" s="96"/>
-      <c r="CP9" s="96"/>
-      <c r="CQ9" s="96"/>
-      <c r="CR9" s="96"/>
-      <c r="CS9" s="96"/>
-      <c r="CT9" s="96"/>
-      <c r="CU9" s="96"/>
-      <c r="CV9" s="96"/>
-      <c r="CW9" s="96"/>
-      <c r="CX9" s="96"/>
-      <c r="CY9" s="96"/>
-      <c r="CZ9" s="96"/>
-      <c r="DA9" s="96"/>
-      <c r="DB9" s="96"/>
-      <c r="DC9" s="96"/>
-      <c r="DD9" s="96"/>
-      <c r="DE9" s="96"/>
-      <c r="DF9" s="96"/>
-      <c r="DG9" s="96"/>
-      <c r="DH9" s="96"/>
-      <c r="DI9" s="96"/>
-      <c r="DJ9" s="96"/>
-      <c r="DK9" s="96"/>
-      <c r="DL9" s="96"/>
-      <c r="DM9" s="96"/>
-      <c r="DN9" s="96"/>
-      <c r="DO9" s="96"/>
-      <c r="DP9" s="96"/>
-      <c r="DQ9" s="96"/>
-      <c r="DR9" s="96"/>
-      <c r="DS9" s="96"/>
-      <c r="DT9" s="96"/>
-      <c r="DU9" s="96"/>
-      <c r="DV9" s="96"/>
-      <c r="DW9" s="96"/>
-      <c r="DX9" s="96"/>
-      <c r="DY9" s="96"/>
-      <c r="DZ9" s="96"/>
-      <c r="EA9" s="96"/>
-      <c r="EB9" s="96"/>
-      <c r="EC9" s="96"/>
-      <c r="ED9" s="96"/>
-      <c r="EE9" s="96"/>
-      <c r="EF9" s="96"/>
-      <c r="EG9" s="96"/>
-      <c r="EH9" s="96"/>
-      <c r="EI9" s="96"/>
-      <c r="EJ9" s="96"/>
-      <c r="EK9" s="96"/>
-      <c r="EL9" s="96"/>
-      <c r="EM9" s="96"/>
-      <c r="EN9" s="96"/>
-      <c r="EO9" s="96"/>
-      <c r="EP9" s="96"/>
-      <c r="EQ9" s="96"/>
-      <c r="ER9" s="96"/>
-      <c r="ES9" s="96"/>
-      <c r="ET9" s="96"/>
-      <c r="EU9" s="96"/>
-      <c r="EV9" s="96"/>
-      <c r="EW9" s="96"/>
-      <c r="EX9" s="96"/>
-      <c r="EY9" s="96"/>
-      <c r="EZ9" s="96"/>
-      <c r="FA9" s="96"/>
-      <c r="FB9" s="96"/>
-      <c r="FC9" s="96"/>
-      <c r="FD9" s="96"/>
-      <c r="FE9" s="96"/>
-      <c r="FF9" s="96"/>
-      <c r="FG9" s="96"/>
-      <c r="FH9" s="96"/>
-      <c r="FI9" s="96"/>
-      <c r="FJ9" s="96"/>
-      <c r="FK9" s="96"/>
-      <c r="FL9" s="96"/>
-      <c r="FM9" s="96"/>
-      <c r="FN9" s="96"/>
-      <c r="FO9" s="96"/>
-      <c r="FP9" s="96"/>
-      <c r="FQ9" s="96"/>
-      <c r="FR9" s="96"/>
-      <c r="FS9" s="96"/>
-      <c r="FT9" s="96"/>
-      <c r="FU9" s="96"/>
-      <c r="FV9" s="96"/>
-      <c r="FW9" s="96"/>
-      <c r="FX9" s="96"/>
-      <c r="FY9" s="96"/>
-      <c r="FZ9" s="96"/>
-      <c r="GA9" s="96"/>
-      <c r="GB9" s="96"/>
-      <c r="GC9" s="96"/>
-      <c r="GD9" s="96"/>
-      <c r="GE9" s="96"/>
-      <c r="GF9" s="96"/>
-      <c r="GG9" s="96"/>
-      <c r="GH9" s="96"/>
-      <c r="GI9" s="96"/>
-      <c r="GJ9" s="96"/>
-      <c r="GK9" s="96"/>
-      <c r="GL9" s="96"/>
-      <c r="GM9" s="96"/>
-      <c r="GN9" s="96"/>
-      <c r="GO9" s="96"/>
-      <c r="GP9" s="96"/>
-      <c r="GQ9" s="96"/>
-      <c r="GR9" s="96"/>
-      <c r="GS9" s="96"/>
-      <c r="GT9" s="96"/>
-      <c r="GU9" s="96"/>
-      <c r="GV9" s="96"/>
-      <c r="GW9" s="96"/>
-      <c r="GX9" s="96"/>
-      <c r="GY9" s="96"/>
-      <c r="GZ9" s="96"/>
-      <c r="HA9" s="96"/>
-      <c r="HB9" s="96"/>
-      <c r="HC9" s="96"/>
-      <c r="HD9" s="96"/>
-      <c r="HE9" s="96"/>
-      <c r="HF9" s="96"/>
-      <c r="HG9" s="96"/>
-      <c r="HH9" s="96"/>
-      <c r="HI9" s="96"/>
-      <c r="HJ9" s="96"/>
-      <c r="HK9" s="96"/>
-      <c r="HL9" s="96"/>
-      <c r="HM9" s="96"/>
-      <c r="HN9" s="96"/>
-      <c r="HO9" s="96"/>
-      <c r="HP9" s="96"/>
-      <c r="HQ9" s="96"/>
-      <c r="HR9" s="96"/>
-      <c r="HS9" s="96"/>
-      <c r="HT9" s="96"/>
-      <c r="HU9" s="96"/>
-      <c r="HV9" s="96"/>
-      <c r="HW9" s="96"/>
-      <c r="HX9" s="96"/>
-      <c r="HY9" s="96"/>
-      <c r="HZ9" s="96"/>
-      <c r="IA9" s="96"/>
-      <c r="IB9" s="96"/>
-      <c r="IC9" s="96"/>
-      <c r="ID9" s="96"/>
-      <c r="IE9" s="96"/>
-      <c r="IF9" s="96"/>
+      <c r="N9" s="84"/>
+      <c r="O9" s="84"/>
+      <c r="P9" s="92"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="93"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="83"/>
+      <c r="AA9" s="83"/>
+      <c r="AB9" s="83"/>
+      <c r="AC9" s="83"/>
+      <c r="AD9" s="83"/>
+      <c r="AE9" s="83"/>
+      <c r="AF9" s="83"/>
+      <c r="AG9" s="83"/>
+      <c r="AH9" s="83"/>
+      <c r="AI9" s="83"/>
+      <c r="AJ9" s="83"/>
+      <c r="AK9" s="83"/>
+      <c r="AL9" s="83"/>
+      <c r="AM9" s="83"/>
+      <c r="AN9" s="83"/>
+      <c r="AO9" s="83"/>
+      <c r="AP9" s="83"/>
+      <c r="AQ9" s="83"/>
+      <c r="AR9" s="83"/>
+      <c r="AS9" s="83"/>
+      <c r="AT9" s="83"/>
+      <c r="AU9" s="83"/>
+      <c r="AV9" s="83"/>
+      <c r="AW9" s="83"/>
+      <c r="AX9" s="83"/>
+      <c r="AY9" s="83"/>
+      <c r="AZ9" s="83"/>
+      <c r="BA9" s="83"/>
+      <c r="BB9" s="83"/>
+      <c r="BC9" s="83"/>
+      <c r="BD9" s="83"/>
+      <c r="BE9" s="83"/>
+      <c r="BF9" s="83"/>
+      <c r="BG9" s="83"/>
+      <c r="BH9" s="83"/>
+      <c r="BI9" s="83"/>
+      <c r="BJ9" s="83"/>
+      <c r="BK9" s="83"/>
+      <c r="BL9" s="83"/>
+      <c r="BM9" s="83"/>
+      <c r="BN9" s="83"/>
+      <c r="BO9" s="83"/>
+      <c r="BP9" s="83"/>
+      <c r="BQ9" s="83"/>
+      <c r="BR9" s="83"/>
+      <c r="BS9" s="83"/>
+      <c r="BT9" s="83"/>
+      <c r="BU9" s="83"/>
+      <c r="BV9" s="83"/>
+      <c r="BW9" s="83"/>
+      <c r="BX9" s="83"/>
+      <c r="BY9" s="83"/>
+      <c r="BZ9" s="83"/>
+      <c r="CA9" s="83"/>
+      <c r="CB9" s="83"/>
+      <c r="CC9" s="83"/>
+      <c r="CD9" s="83"/>
+      <c r="CE9" s="83"/>
+      <c r="CF9" s="83"/>
+      <c r="CG9" s="83"/>
+      <c r="CH9" s="83"/>
+      <c r="CI9" s="83"/>
+      <c r="CJ9" s="83"/>
+      <c r="CK9" s="83"/>
+      <c r="CL9" s="83"/>
+      <c r="CM9" s="83"/>
+      <c r="CN9" s="83"/>
+      <c r="CO9" s="83"/>
+      <c r="CP9" s="83"/>
+      <c r="CQ9" s="83"/>
+      <c r="CR9" s="83"/>
+      <c r="CS9" s="83"/>
+      <c r="CT9" s="83"/>
+      <c r="CU9" s="83"/>
+      <c r="CV9" s="83"/>
+      <c r="CW9" s="83"/>
+      <c r="CX9" s="83"/>
+      <c r="CY9" s="83"/>
+      <c r="CZ9" s="83"/>
+      <c r="DA9" s="83"/>
+      <c r="DB9" s="83"/>
+      <c r="DC9" s="83"/>
+      <c r="DD9" s="83"/>
+      <c r="DE9" s="83"/>
+      <c r="DF9" s="83"/>
+      <c r="DG9" s="83"/>
+      <c r="DH9" s="83"/>
+      <c r="DI9" s="83"/>
+      <c r="DJ9" s="83"/>
+      <c r="DK9" s="83"/>
+      <c r="DL9" s="83"/>
+      <c r="DM9" s="83"/>
+      <c r="DN9" s="83"/>
+      <c r="DO9" s="83"/>
+      <c r="DP9" s="83"/>
+      <c r="DQ9" s="83"/>
+      <c r="DR9" s="83"/>
+      <c r="DS9" s="83"/>
+      <c r="DT9" s="83"/>
+      <c r="DU9" s="83"/>
+      <c r="DV9" s="83"/>
+      <c r="DW9" s="83"/>
+      <c r="DX9" s="83"/>
+      <c r="DY9" s="83"/>
+      <c r="DZ9" s="83"/>
+      <c r="EA9" s="83"/>
+      <c r="EB9" s="83"/>
+      <c r="EC9" s="83"/>
+      <c r="ED9" s="83"/>
+      <c r="EE9" s="83"/>
+      <c r="EF9" s="83"/>
+      <c r="EG9" s="83"/>
+      <c r="EH9" s="83"/>
+      <c r="EI9" s="83"/>
+      <c r="EJ9" s="83"/>
+      <c r="EK9" s="83"/>
+      <c r="EL9" s="83"/>
+      <c r="EM9" s="83"/>
+      <c r="EN9" s="83"/>
+      <c r="EO9" s="83"/>
+      <c r="EP9" s="83"/>
+      <c r="EQ9" s="83"/>
+      <c r="ER9" s="83"/>
+      <c r="ES9" s="83"/>
+      <c r="ET9" s="83"/>
+      <c r="EU9" s="83"/>
+      <c r="EV9" s="83"/>
+      <c r="EW9" s="83"/>
+      <c r="EX9" s="83"/>
+      <c r="EY9" s="83"/>
+      <c r="EZ9" s="83"/>
+      <c r="FA9" s="83"/>
+      <c r="FB9" s="83"/>
+      <c r="FC9" s="83"/>
+      <c r="FD9" s="83"/>
+      <c r="FE9" s="83"/>
+      <c r="FF9" s="83"/>
+      <c r="FG9" s="83"/>
+      <c r="FH9" s="83"/>
+      <c r="FI9" s="83"/>
+      <c r="FJ9" s="83"/>
+      <c r="FK9" s="83"/>
+      <c r="FL9" s="83"/>
+      <c r="FM9" s="83"/>
+      <c r="FN9" s="83"/>
+      <c r="FO9" s="83"/>
+      <c r="FP9" s="83"/>
+      <c r="FQ9" s="83"/>
+      <c r="FR9" s="83"/>
+      <c r="FS9" s="83"/>
+      <c r="FT9" s="83"/>
+      <c r="FU9" s="83"/>
+      <c r="FV9" s="83"/>
+      <c r="FW9" s="83"/>
+      <c r="FX9" s="83"/>
+      <c r="FY9" s="83"/>
+      <c r="FZ9" s="83"/>
+      <c r="GA9" s="83"/>
+      <c r="GB9" s="83"/>
+      <c r="GC9" s="83"/>
+      <c r="GD9" s="83"/>
+      <c r="GE9" s="83"/>
+      <c r="GF9" s="83"/>
+      <c r="GG9" s="83"/>
+      <c r="GH9" s="83"/>
+      <c r="GI9" s="83"/>
+      <c r="GJ9" s="83"/>
+      <c r="GK9" s="83"/>
+      <c r="GL9" s="83"/>
+      <c r="GM9" s="83"/>
+      <c r="GN9" s="83"/>
+      <c r="GO9" s="83"/>
+      <c r="GP9" s="83"/>
+      <c r="GQ9" s="83"/>
+      <c r="GR9" s="83"/>
+      <c r="GS9" s="83"/>
+      <c r="GT9" s="83"/>
+      <c r="GU9" s="83"/>
+      <c r="GV9" s="83"/>
+      <c r="GW9" s="83"/>
+      <c r="GX9" s="83"/>
+      <c r="GY9" s="83"/>
+      <c r="GZ9" s="83"/>
+      <c r="HA9" s="83"/>
+      <c r="HB9" s="83"/>
+      <c r="HC9" s="83"/>
+      <c r="HD9" s="83"/>
+      <c r="HE9" s="83"/>
+      <c r="HF9" s="83"/>
+      <c r="HG9" s="83"/>
+      <c r="HH9" s="83"/>
+      <c r="HI9" s="83"/>
+      <c r="HJ9" s="83"/>
+      <c r="HK9" s="83"/>
+      <c r="HL9" s="83"/>
+      <c r="HM9" s="83"/>
+      <c r="HN9" s="83"/>
+      <c r="HO9" s="83"/>
+      <c r="HP9" s="83"/>
+      <c r="HQ9" s="83"/>
+      <c r="HR9" s="83"/>
+      <c r="HS9" s="83"/>
+      <c r="HT9" s="83"/>
+      <c r="HU9" s="83"/>
+      <c r="HV9" s="83"/>
+      <c r="HW9" s="83"/>
+      <c r="HX9" s="83"/>
+      <c r="HY9" s="83"/>
+      <c r="HZ9" s="83"/>
+      <c r="IA9" s="83"/>
+      <c r="IB9" s="83"/>
+      <c r="IC9" s="83"/>
+      <c r="ID9" s="83"/>
+      <c r="IE9" s="83"/>
+      <c r="IF9" s="83"/>
     </row>
     <row r="10" spans="1:240" x14ac:dyDescent="0.15">
-      <c r="A10" s="98"/>
-      <c r="B10" s="107" t="s">
+      <c r="A10" s="85"/>
+      <c r="B10" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="95" t="s">
         <v>332</v>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="108" t="s">
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="95" t="s">
         <v>333</v>
       </c>
-      <c r="J10" s="108"/>
-      <c r="K10" s="110">
+      <c r="J10" s="95"/>
+      <c r="K10" s="97">
         <v>1</v>
       </c>
-      <c r="L10" s="108" t="s">
+      <c r="L10" s="95" t="s">
         <v>334</v>
       </c>
-      <c r="M10" s="108" t="s">
+      <c r="M10" s="95" t="s">
         <v>335</v>
       </c>
-      <c r="N10" s="97"/>
-      <c r="O10" s="97"/>
-      <c r="P10" s="105"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="106"/>
-      <c r="S10" s="106"/>
-      <c r="T10" s="96"/>
-      <c r="U10" s="96"/>
-      <c r="V10" s="96"/>
-      <c r="W10" s="96"/>
-      <c r="X10" s="96"/>
-      <c r="Y10" s="96"/>
-      <c r="Z10" s="96"/>
-      <c r="AA10" s="96"/>
-      <c r="AB10" s="96"/>
-      <c r="AC10" s="96"/>
-      <c r="AD10" s="96"/>
-      <c r="AE10" s="96"/>
-      <c r="AF10" s="96"/>
-      <c r="AG10" s="96"/>
-      <c r="AH10" s="96"/>
-      <c r="AI10" s="96"/>
-      <c r="AJ10" s="96"/>
-      <c r="AK10" s="96"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="96"/>
-      <c r="AN10" s="96"/>
-      <c r="AO10" s="96"/>
-      <c r="AP10" s="96"/>
-      <c r="AQ10" s="96"/>
-      <c r="AR10" s="96"/>
-      <c r="AS10" s="96"/>
-      <c r="AT10" s="96"/>
-      <c r="AU10" s="96"/>
-      <c r="AV10" s="96"/>
-      <c r="AW10" s="96"/>
-      <c r="AX10" s="96"/>
-      <c r="AY10" s="96"/>
-      <c r="AZ10" s="96"/>
-      <c r="BA10" s="96"/>
-      <c r="BB10" s="96"/>
-      <c r="BC10" s="96"/>
-      <c r="BD10" s="96"/>
-      <c r="BE10" s="96"/>
-      <c r="BF10" s="96"/>
-      <c r="BG10" s="96"/>
-      <c r="BH10" s="96"/>
-      <c r="BI10" s="96"/>
-      <c r="BJ10" s="96"/>
-      <c r="BK10" s="96"/>
-      <c r="BL10" s="96"/>
-      <c r="BM10" s="96"/>
-      <c r="BN10" s="96"/>
-      <c r="BO10" s="96"/>
-      <c r="BP10" s="96"/>
-      <c r="BQ10" s="96"/>
-      <c r="BR10" s="96"/>
-      <c r="BS10" s="96"/>
-      <c r="BT10" s="96"/>
-      <c r="BU10" s="96"/>
-      <c r="BV10" s="96"/>
-      <c r="BW10" s="96"/>
-      <c r="BX10" s="96"/>
-      <c r="BY10" s="96"/>
-      <c r="BZ10" s="96"/>
-      <c r="CA10" s="96"/>
-      <c r="CB10" s="96"/>
-      <c r="CC10" s="96"/>
-      <c r="CD10" s="96"/>
-      <c r="CE10" s="96"/>
-      <c r="CF10" s="96"/>
-      <c r="CG10" s="96"/>
-      <c r="CH10" s="96"/>
-      <c r="CI10" s="96"/>
-      <c r="CJ10" s="96"/>
-      <c r="CK10" s="96"/>
-      <c r="CL10" s="96"/>
-      <c r="CM10" s="96"/>
-      <c r="CN10" s="96"/>
-      <c r="CO10" s="96"/>
-      <c r="CP10" s="96"/>
-      <c r="CQ10" s="96"/>
-      <c r="CR10" s="96"/>
-      <c r="CS10" s="96"/>
-      <c r="CT10" s="96"/>
-      <c r="CU10" s="96"/>
-      <c r="CV10" s="96"/>
-      <c r="CW10" s="96"/>
-      <c r="CX10" s="96"/>
-      <c r="CY10" s="96"/>
-      <c r="CZ10" s="96"/>
-      <c r="DA10" s="96"/>
-      <c r="DB10" s="96"/>
-      <c r="DC10" s="96"/>
-      <c r="DD10" s="96"/>
-      <c r="DE10" s="96"/>
-      <c r="DF10" s="96"/>
-      <c r="DG10" s="96"/>
-      <c r="DH10" s="96"/>
-      <c r="DI10" s="96"/>
-      <c r="DJ10" s="96"/>
-      <c r="DK10" s="96"/>
-      <c r="DL10" s="96"/>
-      <c r="DM10" s="96"/>
-      <c r="DN10" s="96"/>
-      <c r="DO10" s="96"/>
-      <c r="DP10" s="96"/>
-      <c r="DQ10" s="96"/>
-      <c r="DR10" s="96"/>
-      <c r="DS10" s="96"/>
-      <c r="DT10" s="96"/>
-      <c r="DU10" s="96"/>
-      <c r="DV10" s="96"/>
-      <c r="DW10" s="96"/>
-      <c r="DX10" s="96"/>
-      <c r="DY10" s="96"/>
-      <c r="DZ10" s="96"/>
-      <c r="EA10" s="96"/>
-      <c r="EB10" s="96"/>
-      <c r="EC10" s="96"/>
-      <c r="ED10" s="96"/>
-      <c r="EE10" s="96"/>
-      <c r="EF10" s="96"/>
-      <c r="EG10" s="96"/>
-      <c r="EH10" s="96"/>
-      <c r="EI10" s="96"/>
-      <c r="EJ10" s="96"/>
-      <c r="EK10" s="96"/>
-      <c r="EL10" s="96"/>
-      <c r="EM10" s="96"/>
-      <c r="EN10" s="96"/>
-      <c r="EO10" s="96"/>
-      <c r="EP10" s="96"/>
-      <c r="EQ10" s="96"/>
-      <c r="ER10" s="96"/>
-      <c r="ES10" s="96"/>
-      <c r="ET10" s="96"/>
-      <c r="EU10" s="96"/>
-      <c r="EV10" s="96"/>
-      <c r="EW10" s="96"/>
-      <c r="EX10" s="96"/>
-      <c r="EY10" s="96"/>
-      <c r="EZ10" s="96"/>
-      <c r="FA10" s="96"/>
-      <c r="FB10" s="96"/>
-      <c r="FC10" s="96"/>
-      <c r="FD10" s="96"/>
-      <c r="FE10" s="96"/>
-      <c r="FF10" s="96"/>
-      <c r="FG10" s="96"/>
-      <c r="FH10" s="96"/>
-      <c r="FI10" s="96"/>
-      <c r="FJ10" s="96"/>
-      <c r="FK10" s="96"/>
-      <c r="FL10" s="96"/>
-      <c r="FM10" s="96"/>
-      <c r="FN10" s="96"/>
-      <c r="FO10" s="96"/>
-      <c r="FP10" s="96"/>
-      <c r="FQ10" s="96"/>
-      <c r="FR10" s="96"/>
-      <c r="FS10" s="96"/>
-      <c r="FT10" s="96"/>
-      <c r="FU10" s="96"/>
-      <c r="FV10" s="96"/>
-      <c r="FW10" s="96"/>
-      <c r="FX10" s="96"/>
-      <c r="FY10" s="96"/>
-      <c r="FZ10" s="96"/>
-      <c r="GA10" s="96"/>
-      <c r="GB10" s="96"/>
-      <c r="GC10" s="96"/>
-      <c r="GD10" s="96"/>
-      <c r="GE10" s="96"/>
-      <c r="GF10" s="96"/>
-      <c r="GG10" s="96"/>
-      <c r="GH10" s="96"/>
-      <c r="GI10" s="96"/>
-      <c r="GJ10" s="96"/>
-      <c r="GK10" s="96"/>
-      <c r="GL10" s="96"/>
-      <c r="GM10" s="96"/>
-      <c r="GN10" s="96"/>
-      <c r="GO10" s="96"/>
-      <c r="GP10" s="96"/>
-      <c r="GQ10" s="96"/>
-      <c r="GR10" s="96"/>
-      <c r="GS10" s="96"/>
-      <c r="GT10" s="96"/>
-      <c r="GU10" s="96"/>
-      <c r="GV10" s="96"/>
-      <c r="GW10" s="96"/>
-      <c r="GX10" s="96"/>
-      <c r="GY10" s="96"/>
-      <c r="GZ10" s="96"/>
-      <c r="HA10" s="96"/>
-      <c r="HB10" s="96"/>
-      <c r="HC10" s="96"/>
-      <c r="HD10" s="96"/>
-      <c r="HE10" s="96"/>
-      <c r="HF10" s="96"/>
-      <c r="HG10" s="96"/>
-      <c r="HH10" s="96"/>
-      <c r="HI10" s="96"/>
-      <c r="HJ10" s="96"/>
-      <c r="HK10" s="96"/>
-      <c r="HL10" s="96"/>
-      <c r="HM10" s="96"/>
-      <c r="HN10" s="96"/>
-      <c r="HO10" s="96"/>
-      <c r="HP10" s="96"/>
-      <c r="HQ10" s="96"/>
-      <c r="HR10" s="96"/>
-      <c r="HS10" s="96"/>
-      <c r="HT10" s="96"/>
-      <c r="HU10" s="96"/>
-      <c r="HV10" s="96"/>
-      <c r="HW10" s="96"/>
-      <c r="HX10" s="96"/>
-      <c r="HY10" s="96"/>
-      <c r="HZ10" s="96"/>
-      <c r="IA10" s="96"/>
-      <c r="IB10" s="96"/>
-      <c r="IC10" s="96"/>
-      <c r="ID10" s="96"/>
-      <c r="IE10" s="96"/>
-      <c r="IF10" s="96"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="92"/>
+      <c r="Q10" s="93"/>
+      <c r="R10" s="93"/>
+      <c r="S10" s="93"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="83"/>
+      <c r="AA10" s="83"/>
+      <c r="AB10" s="83"/>
+      <c r="AC10" s="83"/>
+      <c r="AD10" s="83"/>
+      <c r="AE10" s="83"/>
+      <c r="AF10" s="83"/>
+      <c r="AG10" s="83"/>
+      <c r="AH10" s="83"/>
+      <c r="AI10" s="83"/>
+      <c r="AJ10" s="83"/>
+      <c r="AK10" s="83"/>
+      <c r="AL10" s="83"/>
+      <c r="AM10" s="83"/>
+      <c r="AN10" s="83"/>
+      <c r="AO10" s="83"/>
+      <c r="AP10" s="83"/>
+      <c r="AQ10" s="83"/>
+      <c r="AR10" s="83"/>
+      <c r="AS10" s="83"/>
+      <c r="AT10" s="83"/>
+      <c r="AU10" s="83"/>
+      <c r="AV10" s="83"/>
+      <c r="AW10" s="83"/>
+      <c r="AX10" s="83"/>
+      <c r="AY10" s="83"/>
+      <c r="AZ10" s="83"/>
+      <c r="BA10" s="83"/>
+      <c r="BB10" s="83"/>
+      <c r="BC10" s="83"/>
+      <c r="BD10" s="83"/>
+      <c r="BE10" s="83"/>
+      <c r="BF10" s="83"/>
+      <c r="BG10" s="83"/>
+      <c r="BH10" s="83"/>
+      <c r="BI10" s="83"/>
+      <c r="BJ10" s="83"/>
+      <c r="BK10" s="83"/>
+      <c r="BL10" s="83"/>
+      <c r="BM10" s="83"/>
+      <c r="BN10" s="83"/>
+      <c r="BO10" s="83"/>
+      <c r="BP10" s="83"/>
+      <c r="BQ10" s="83"/>
+      <c r="BR10" s="83"/>
+      <c r="BS10" s="83"/>
+      <c r="BT10" s="83"/>
+      <c r="BU10" s="83"/>
+      <c r="BV10" s="83"/>
+      <c r="BW10" s="83"/>
+      <c r="BX10" s="83"/>
+      <c r="BY10" s="83"/>
+      <c r="BZ10" s="83"/>
+      <c r="CA10" s="83"/>
+      <c r="CB10" s="83"/>
+      <c r="CC10" s="83"/>
+      <c r="CD10" s="83"/>
+      <c r="CE10" s="83"/>
+      <c r="CF10" s="83"/>
+      <c r="CG10" s="83"/>
+      <c r="CH10" s="83"/>
+      <c r="CI10" s="83"/>
+      <c r="CJ10" s="83"/>
+      <c r="CK10" s="83"/>
+      <c r="CL10" s="83"/>
+      <c r="CM10" s="83"/>
+      <c r="CN10" s="83"/>
+      <c r="CO10" s="83"/>
+      <c r="CP10" s="83"/>
+      <c r="CQ10" s="83"/>
+      <c r="CR10" s="83"/>
+      <c r="CS10" s="83"/>
+      <c r="CT10" s="83"/>
+      <c r="CU10" s="83"/>
+      <c r="CV10" s="83"/>
+      <c r="CW10" s="83"/>
+      <c r="CX10" s="83"/>
+      <c r="CY10" s="83"/>
+      <c r="CZ10" s="83"/>
+      <c r="DA10" s="83"/>
+      <c r="DB10" s="83"/>
+      <c r="DC10" s="83"/>
+      <c r="DD10" s="83"/>
+      <c r="DE10" s="83"/>
+      <c r="DF10" s="83"/>
+      <c r="DG10" s="83"/>
+      <c r="DH10" s="83"/>
+      <c r="DI10" s="83"/>
+      <c r="DJ10" s="83"/>
+      <c r="DK10" s="83"/>
+      <c r="DL10" s="83"/>
+      <c r="DM10" s="83"/>
+      <c r="DN10" s="83"/>
+      <c r="DO10" s="83"/>
+      <c r="DP10" s="83"/>
+      <c r="DQ10" s="83"/>
+      <c r="DR10" s="83"/>
+      <c r="DS10" s="83"/>
+      <c r="DT10" s="83"/>
+      <c r="DU10" s="83"/>
+      <c r="DV10" s="83"/>
+      <c r="DW10" s="83"/>
+      <c r="DX10" s="83"/>
+      <c r="DY10" s="83"/>
+      <c r="DZ10" s="83"/>
+      <c r="EA10" s="83"/>
+      <c r="EB10" s="83"/>
+      <c r="EC10" s="83"/>
+      <c r="ED10" s="83"/>
+      <c r="EE10" s="83"/>
+      <c r="EF10" s="83"/>
+      <c r="EG10" s="83"/>
+      <c r="EH10" s="83"/>
+      <c r="EI10" s="83"/>
+      <c r="EJ10" s="83"/>
+      <c r="EK10" s="83"/>
+      <c r="EL10" s="83"/>
+      <c r="EM10" s="83"/>
+      <c r="EN10" s="83"/>
+      <c r="EO10" s="83"/>
+      <c r="EP10" s="83"/>
+      <c r="EQ10" s="83"/>
+      <c r="ER10" s="83"/>
+      <c r="ES10" s="83"/>
+      <c r="ET10" s="83"/>
+      <c r="EU10" s="83"/>
+      <c r="EV10" s="83"/>
+      <c r="EW10" s="83"/>
+      <c r="EX10" s="83"/>
+      <c r="EY10" s="83"/>
+      <c r="EZ10" s="83"/>
+      <c r="FA10" s="83"/>
+      <c r="FB10" s="83"/>
+      <c r="FC10" s="83"/>
+      <c r="FD10" s="83"/>
+      <c r="FE10" s="83"/>
+      <c r="FF10" s="83"/>
+      <c r="FG10" s="83"/>
+      <c r="FH10" s="83"/>
+      <c r="FI10" s="83"/>
+      <c r="FJ10" s="83"/>
+      <c r="FK10" s="83"/>
+      <c r="FL10" s="83"/>
+      <c r="FM10" s="83"/>
+      <c r="FN10" s="83"/>
+      <c r="FO10" s="83"/>
+      <c r="FP10" s="83"/>
+      <c r="FQ10" s="83"/>
+      <c r="FR10" s="83"/>
+      <c r="FS10" s="83"/>
+      <c r="FT10" s="83"/>
+      <c r="FU10" s="83"/>
+      <c r="FV10" s="83"/>
+      <c r="FW10" s="83"/>
+      <c r="FX10" s="83"/>
+      <c r="FY10" s="83"/>
+      <c r="FZ10" s="83"/>
+      <c r="GA10" s="83"/>
+      <c r="GB10" s="83"/>
+      <c r="GC10" s="83"/>
+      <c r="GD10" s="83"/>
+      <c r="GE10" s="83"/>
+      <c r="GF10" s="83"/>
+      <c r="GG10" s="83"/>
+      <c r="GH10" s="83"/>
+      <c r="GI10" s="83"/>
+      <c r="GJ10" s="83"/>
+      <c r="GK10" s="83"/>
+      <c r="GL10" s="83"/>
+      <c r="GM10" s="83"/>
+      <c r="GN10" s="83"/>
+      <c r="GO10" s="83"/>
+      <c r="GP10" s="83"/>
+      <c r="GQ10" s="83"/>
+      <c r="GR10" s="83"/>
+      <c r="GS10" s="83"/>
+      <c r="GT10" s="83"/>
+      <c r="GU10" s="83"/>
+      <c r="GV10" s="83"/>
+      <c r="GW10" s="83"/>
+      <c r="GX10" s="83"/>
+      <c r="GY10" s="83"/>
+      <c r="GZ10" s="83"/>
+      <c r="HA10" s="83"/>
+      <c r="HB10" s="83"/>
+      <c r="HC10" s="83"/>
+      <c r="HD10" s="83"/>
+      <c r="HE10" s="83"/>
+      <c r="HF10" s="83"/>
+      <c r="HG10" s="83"/>
+      <c r="HH10" s="83"/>
+      <c r="HI10" s="83"/>
+      <c r="HJ10" s="83"/>
+      <c r="HK10" s="83"/>
+      <c r="HL10" s="83"/>
+      <c r="HM10" s="83"/>
+      <c r="HN10" s="83"/>
+      <c r="HO10" s="83"/>
+      <c r="HP10" s="83"/>
+      <c r="HQ10" s="83"/>
+      <c r="HR10" s="83"/>
+      <c r="HS10" s="83"/>
+      <c r="HT10" s="83"/>
+      <c r="HU10" s="83"/>
+      <c r="HV10" s="83"/>
+      <c r="HW10" s="83"/>
+      <c r="HX10" s="83"/>
+      <c r="HY10" s="83"/>
+      <c r="HZ10" s="83"/>
+      <c r="IA10" s="83"/>
+      <c r="IB10" s="83"/>
+      <c r="IC10" s="83"/>
+      <c r="ID10" s="83"/>
+      <c r="IE10" s="83"/>
+      <c r="IF10" s="83"/>
     </row>
     <row r="11" spans="1:240" x14ac:dyDescent="0.15">
       <c r="B11" s="16"/>
@@ -43243,7 +43243,7 @@
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="73" t="s">
         <v>237</v>
       </c>
       <c r="D2" s="8"/>
@@ -43276,7 +43276,7 @@
       <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="73" t="s">
         <v>301</v>
       </c>
       <c r="D3" s="8"/>
@@ -43405,7 +43405,7 @@
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="73" t="s">
         <v>303</v>
       </c>
       <c r="D7" s="8"/>
@@ -43493,17 +43493,17 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="102" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="77"/>
-      <c r="H10" s="78"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="104"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -43526,23 +43526,23 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="83" t="s">
+      <c r="D11" s="108"/>
+      <c r="E11" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="84" t="s">
+      <c r="F11" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="84" t="s">
+      <c r="G11" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="84" t="s">
+      <c r="H11" s="110" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="4"/>
@@ -43567,17 +43567,17 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
-      <c r="B12" s="80"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
+      <c r="E12" s="108"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>

</xml_diff>